<commit_message>
Start ProjectPlan; Separate UserStories from Readme
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Heidi Local Files\0_MATC_CURRENT\EnterpriseJava\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB04D541-1A85-48A4-8EAC-6ADAB2A29069}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED91C8E-F3BE-4DBE-A509-3CDD48BE5CA8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11700" windowHeight="9735" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -76,14 +76,40 @@
   </si>
   <si>
     <t>Week 2: Exercise overview, week 2 reading.  Project: more work on problem statement.</t>
+  </si>
+  <si>
+    <t>Watched part of Ex 1 solution; Worked on Ex 2 and cleaning up activities for Week 2.</t>
+  </si>
+  <si>
+    <t>Worked on Exercise 2</t>
+  </si>
+  <si>
+    <t>Reworked Ex. 2 to make return values more unique for exceptions in order to prove exception handling. Attempted refactor but it would've really messed up tests (too much to recover from today).  Completed Week 3 videos, demo activity, and reading.</t>
+  </si>
+  <si>
+    <t>Indie Project: Worked on project layouts and reviewed Zillow API options more carefully - looks like it won't do what I want it to do after all.</t>
+  </si>
+  <si>
+    <t>Indie Project: Continued work on layouts; decided to expand intake survey and save the financial story as the only "level up" step</t>
+  </si>
+  <si>
+    <t>Indie Project: Worked on user stories, looked into wireframe tools, signed up for student account on Moqup, and continued setting up ideas for what should be on each web page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,10 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -431,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,19 +472,20 @@
     <col min="4" max="4" width="114.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -577,6 +608,72 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43502</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43503</v>
+      </c>
+      <c r="B16">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43507</v>
+      </c>
+      <c r="B17">
+        <v>5.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43509</v>
+      </c>
+      <c r="B18">
+        <v>3.5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43511</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43512</v>
+      </c>
+      <c r="B20">
+        <v>4.5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds project plan through 3/4 closely following sample plan
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED91C8E-F3BE-4DBE-A509-3CDD48BE5CA8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E72940D-0ADE-4A0E-A379-FE19AF42877C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Indie Project: Worked on user stories, looked into wireframe tools, signed up for student account on Moqup, and continued setting up ideas for what should be on each web page.</t>
+  </si>
+  <si>
+    <t>5:10 - 6:50 Sunday: Started project plan, revised user stories and separated them from readme</t>
+  </si>
+  <si>
+    <t>7:20 -  9:10 Week 4: Intro video; browsing tech topics…. Idea: would Hibernate Search help an administrator scan text entries?  Or help users scan the forum for mentions? Continued project plan.</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,6 +682,16 @@
         <v>21</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Provides an initial project plan through completion
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E72940D-0ADE-4A0E-A379-FE19AF42877C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2E0C4-1D6F-49A7-9C4E-38EE276394D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>7:20 -  9:10 Week 4: Intro video; browsing tech topics…. Idea: would Hibernate Search help an administrator scan text entries?  Or help users scan the forum for mentions? Continued project plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3pm - </t>
+  </si>
+  <si>
+    <t>Need to: make layout for forum, thread</t>
+  </si>
+  <si>
+    <t>Need to decide about abilities and presentation for admin</t>
+  </si>
+  <si>
+    <t>Need to revise intro and probably user stories to reflect evolution here.</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,6 +704,26 @@
         <v>24</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adds page designs for initial scope except forum and admin
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2E0C4-1D6F-49A7-9C4E-38EE276394D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31449A08-7026-4824-B7C4-94D3DE1896C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -102,16 +102,13 @@
     <t>7:20 -  9:10 Week 4: Intro video; browsing tech topics…. Idea: would Hibernate Search help an administrator scan text entries?  Or help users scan the forum for mentions? Continued project plan.</t>
   </si>
   <si>
-    <t xml:space="preserve">3pm - </t>
-  </si>
-  <si>
-    <t>Need to: make layout for forum, thread</t>
-  </si>
-  <si>
-    <t>Need to decide about abilities and presentation for admin</t>
-  </si>
-  <si>
-    <t>Need to revise intro and probably user stories to reflect evolution here.</t>
+    <t>Need to decide about abilities and presentation for admin --- probably same views but with some kind of ability to see "removed content" stats, and with edit/remove options in more places.</t>
+  </si>
+  <si>
+    <t>Need to: make layout for forum, thread, admin view of questionable users</t>
+  </si>
+  <si>
+    <t>3pm - 4:45 Revised project plan, user stories, and project plan to reflect current status.</t>
   </si>
 </sst>
 </file>
@@ -479,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +703,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,14 +711,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds Forum and Admin Designs
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31449A08-7026-4824-B7C4-94D3DE1896C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391748D9-3D3E-4817-8715-61DB9A33F0A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -102,13 +102,10 @@
     <t>7:20 -  9:10 Week 4: Intro video; browsing tech topics…. Idea: would Hibernate Search help an administrator scan text entries?  Or help users scan the forum for mentions? Continued project plan.</t>
   </si>
   <si>
-    <t>Need to decide about abilities and presentation for admin --- probably same views but with some kind of ability to see "removed content" stats, and with edit/remove options in more places.</t>
-  </si>
-  <si>
-    <t>Need to: make layout for forum, thread, admin view of questionable users</t>
-  </si>
-  <si>
     <t>3pm - 4:45 Revised project plan, user stories, and project plan to reflect current status.</t>
+  </si>
+  <si>
+    <t>8:30 -10 Completed page designs for current scope</t>
   </si>
 </sst>
 </file>
@@ -476,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,17 +700,12 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempts link fixes in README; updates time log through 2/17
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391748D9-3D3E-4817-8715-61DB9A33F0A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A50C2-860D-46AA-8CF7-2C9F5F14A9EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -96,16 +96,7 @@
     <t>Indie Project: Worked on user stories, looked into wireframe tools, signed up for student account on Moqup, and continued setting up ideas for what should be on each web page.</t>
   </si>
   <si>
-    <t>5:10 - 6:50 Sunday: Started project plan, revised user stories and separated them from readme</t>
-  </si>
-  <si>
-    <t>7:20 -  9:10 Week 4: Intro video; browsing tech topics…. Idea: would Hibernate Search help an administrator scan text entries?  Or help users scan the forum for mentions? Continued project plan.</t>
-  </si>
-  <si>
-    <t>3pm - 4:45 Revised project plan, user stories, and project plan to reflect current status.</t>
-  </si>
-  <si>
-    <t>8:30 -10 Completed page designs for current scope</t>
+    <t>Indie Project: Revised user stories and problem statement; finished screen designs; added work to GitHub and appropriate links to README.  Week 4: Watched intro video.  Professional Development: signed up to present on Hibernate Search; also, will this help users search across forums or perhaps across site?  Would it make admin related tasks easier?</t>
   </si>
 </sst>
 </file>
@@ -473,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D29" sqref="D24:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,25 +679,19 @@
         <v>21</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43513</v>
+      </c>
+      <c r="B21">
+        <v>6.5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completes draft ApplicationFlow; Adds user stories re: flagging content
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A50C2-860D-46AA-8CF7-2C9F5F14A9EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBDAB9B-E2A1-481D-938C-7F3BCA2DF13C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1425" windowWidth="20895" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="13575" yWindow="1425" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -97,6 +97,54 @@
   </si>
   <si>
     <t>Indie Project: Revised user stories and problem statement; finished screen designs; added work to GitHub and appropriate links to README.  Week 4: Watched intro video.  Professional Development: signed up to present on Hibernate Search; also, will this help users search across forums or perhaps across site?  Would it make admin related tasks easier?</t>
+  </si>
+  <si>
+    <t>Mon Am 45 min starting app flow</t>
+  </si>
+  <si>
+    <t>15 min dao video reference cave of coding</t>
+  </si>
+  <si>
+    <t>11:50 - flow</t>
+  </si>
+  <si>
+    <t>Need to</t>
+  </si>
+  <si>
+    <t>Revise search interface and flow to match.</t>
+  </si>
+  <si>
+    <t>How will event be triggered to search for matching careers?</t>
+  </si>
+  <si>
+    <t>How will event  be triggered to select matching career and get the median income?</t>
+  </si>
+  <si>
+    <t>Let's skilp the income populating on the form and just show it in the results.</t>
+  </si>
+  <si>
+    <t>Paragraph or summary needs to show user what career they searched on (if they did), what the median income is, and</t>
+  </si>
+  <si>
+    <t>all the other stuff already mentioned in diagram.</t>
+  </si>
+  <si>
+    <t>Need to be consistent across flow/user stories/screens about which capabilities are given to people with simple survey profiles</t>
+  </si>
+  <si>
+    <t>and which are only for those who have written their story.</t>
+  </si>
+  <si>
+    <t>Maybe users have read-only access to everything until they have written their story?</t>
+  </si>
+  <si>
+    <t>Or maybe they only see charts in search and have read-only access to forums?</t>
+  </si>
+  <si>
+    <t>Need a way to go back to the thread list after viewing a specific thread.</t>
+  </si>
+  <si>
+    <t>Add sitewide search function for special topic, maybe on nav bar for signed in users.</t>
   </si>
 </sst>
 </file>
@@ -464,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D24:D29"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,6 +741,86 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates time log for checkpoint 1; accounts for some gaps in plans and technologies
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBDAB9B-E2A1-481D-938C-7F3BCA2DF13C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC287F6-0854-4610-9C0A-C31071A9D7BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13575" yWindow="1425" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -99,52 +99,7 @@
     <t>Indie Project: Revised user stories and problem statement; finished screen designs; added work to GitHub and appropriate links to README.  Week 4: Watched intro video.  Professional Development: signed up to present on Hibernate Search; also, will this help users search across forums or perhaps across site?  Would it make admin related tasks easier?</t>
   </si>
   <si>
-    <t>Mon Am 45 min starting app flow</t>
-  </si>
-  <si>
-    <t>15 min dao video reference cave of coding</t>
-  </si>
-  <si>
-    <t>11:50 - flow</t>
-  </si>
-  <si>
-    <t>Need to</t>
-  </si>
-  <si>
-    <t>Revise search interface and flow to match.</t>
-  </si>
-  <si>
-    <t>How will event be triggered to search for matching careers?</t>
-  </si>
-  <si>
-    <t>How will event  be triggered to select matching career and get the median income?</t>
-  </si>
-  <si>
-    <t>Let's skilp the income populating on the form and just show it in the results.</t>
-  </si>
-  <si>
-    <t>Paragraph or summary needs to show user what career they searched on (if they did), what the median income is, and</t>
-  </si>
-  <si>
-    <t>all the other stuff already mentioned in diagram.</t>
-  </si>
-  <si>
-    <t>Need to be consistent across flow/user stories/screens about which capabilities are given to people with simple survey profiles</t>
-  </si>
-  <si>
-    <t>and which are only for those who have written their story.</t>
-  </si>
-  <si>
-    <t>Maybe users have read-only access to everything until they have written their story?</t>
-  </si>
-  <si>
-    <t>Or maybe they only see charts in search and have read-only access to forums?</t>
-  </si>
-  <si>
-    <t>Need a way to go back to the thread list after viewing a specific thread.</t>
-  </si>
-  <si>
-    <t>Add sitewide search function for special topic, maybe on nav bar for signed in users.</t>
+    <t>Indie Project: Drafted application flow and adapted PW's technologies list to my project; linked both to readme.  Week 4: watched DAO video from reference section (Cave of Coding).</t>
   </si>
 </sst>
 </file>
@@ -512,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,87 +693,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43514</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reflects Checkpoint 1 Feedback in UserStories and ProjectPlan
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC287F6-0854-4610-9C0A-C31071A9D7BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2042BB72-0D00-4D10-94A0-85C1C010E352}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t>Indie Project: Drafted application flow and adapted PW's technologies list to my project; linked both to readme.  Week 4: watched DAO video from reference section (Cave of Coding).</t>
+  </si>
+  <si>
+    <t>Week 4: Worked on demo videos</t>
+  </si>
+  <si>
+    <t>Thurs AM worked on demo videos &lt; 1 hour.</t>
+  </si>
+  <si>
+    <t>plus 2 hrs - some challenges reconciling my project w/diffs w/PW's</t>
+  </si>
+  <si>
+    <t>plus 1 hour finishing demo and working on activity 1 - not sure how to get path for data dump right?</t>
+  </si>
+  <si>
+    <t>NOT RESOLVED: getting correct path for mysqldump (don't need to do it yet so defering…)</t>
+  </si>
+  <si>
+    <t>1:30 -x continue week 4 focused on readings (increasingly skimming hibernate tutorial)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,6 +722,42 @@
         <v>24</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43516</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adds ERD for MVP and Annual Survey user story
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2042BB72-0D00-4D10-94A0-85C1C010E352}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B306EC2-D63B-40B2-9CD1-CE5C4DCBFF70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="2340" yWindow="2415" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -105,19 +105,11 @@
     <t>Week 4: Worked on demo videos</t>
   </si>
   <si>
-    <t>Thurs AM worked on demo videos &lt; 1 hour.</t>
-  </si>
-  <si>
-    <t>plus 2 hrs - some challenges reconciling my project w/diffs w/PW's</t>
-  </si>
-  <si>
-    <t>plus 1 hour finishing demo and working on activity 1 - not sure how to get path for data dump right?</t>
-  </si>
-  <si>
     <t>NOT RESOLVED: getting correct path for mysqldump (don't need to do it yet so defering…)</t>
   </si>
   <si>
-    <t>1:30 -x continue week 4 focused on readings (increasingly skimming hibernate tutorial)</t>
+    <t>Week 4: Finished demo videos, Activity 1, and reading.
+Indie Project: Prioritized User Stories and added tech suggestions to plans.</t>
   </si>
 </sst>
 </file>
@@ -485,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,29 +725,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="s">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43517</v>
+      </c>
+      <c r="B24">
+        <v>5.5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds draft User DAO and SessionFactoryProvider (as provided in coursework)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B306EC2-D63B-40B2-9CD1-CE5C4DCBFF70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4188526E-235C-4ADB-9145-F20D1A00123D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2415" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -110,6 +110,12 @@
   <si>
     <t>Week 4: Finished demo videos, Activity 1, and reading.
 Indie Project: Prioritized User Stories and added tech suggestions to plans.</t>
+  </si>
+  <si>
+    <t>Indie Project: MVP ERD, populated lookup tables, tried to figure mysqldump (saved creation &amp; insert files separately for now), created User entity</t>
+  </si>
+  <si>
+    <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,9 +742,25 @@
         <v>27</v>
       </c>
     </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43518</v>
+      </c>
+      <c r="B25">
+        <v>5.5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaces retrieval method with one that's by generic property name
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4188526E-235C-4ADB-9145-F20D1A00123D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA8D488-A971-4C87-B550-294EDF6EF9EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -112,10 +112,10 @@
 Indie Project: Prioritized User Stories and added tech suggestions to plans.</t>
   </si>
   <si>
-    <t>Indie Project: MVP ERD, populated lookup tables, tried to figure mysqldump (saved creation &amp; insert files separately for now), created User entity</t>
-  </si>
-  <si>
     <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose</t>
+  </si>
+  <si>
+    <t>Indie Project: MVP ERD, populated lookup tables, tried to figure mysqldump (saved creation &amp; insert files separately for now), created User entity and draft dao, copied in SessionFactoryProvider</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,10 +747,10 @@
         <v>43518</v>
       </c>
       <c r="B25">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Has a cleandb.sql that executes completely
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA8D488-A971-4C87-B550-294EDF6EF9EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843FFAFB-3090-4432-8920-FE85FB29B6FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Indie Project: MVP ERD, populated lookup tables, tried to figure mysqldump (saved creation &amp; insert files separately for now), created User entity and draft dao, copied in SessionFactoryProvider</t>
+  </si>
+  <si>
+    <t>Indie Project: setting up test database, properties, copying Database class, creating sql for cleaning database before testing, starting UserDaoTest</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +756,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43519</v>
+      </c>
+      <c r="B26">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
cleandb.sql is readable by Database; passes UserDaoTest addSuccess(); adds hibernate.log to .gitignore
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F948981F-01B2-4A3B-BBA6-9047A3A47D79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273D8268-C877-4A3A-A512-EC013B516A38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -121,13 +121,22 @@
     <t>I have a log4j problem about renaming with the date etc, appears to be the same in week 1 exercise and project.</t>
   </si>
   <si>
-    <t>Indie Project: setting up test database, properties, copying Database class, creating sql for cleaning database before testing, starting UserDaoTest, setting up log4j properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accidently saved pws to github.  Need to change pw and remove files. </t>
-  </si>
-  <si>
-    <t>7:40-X</t>
+    <t>Indie Project: setting up test database, properties, copying Database class, creating sql for cleaning database before testing, starting UserDaoTest, setting up log4j properties, changing mysql username and pw, trying to delete sensitive files from GitHub, troubleshooting why my cleandb.sql isn't actually running...</t>
+  </si>
+  <si>
+    <t>NB: new password so files/setup need to change in prior repos</t>
+  </si>
+  <si>
+    <t>WHY won't cleandb.sql run in my project?</t>
+  </si>
+  <si>
+    <t>Sun AM - 1 hr</t>
+  </si>
+  <si>
+    <t>Week 4ish: Getting passwords out of repo for Week 1 exercise with intention to figure out why this project reads cleandb.sql and it doesn't get read in my project tests</t>
+  </si>
+  <si>
+    <t>NEXT: remove logs from github -- they currently only have the removed user/password</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,40 +774,58 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43519</v>
       </c>
       <c r="B26">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="s">
-        <v>26</v>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43520</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds Javadoc comments and Test Results/Coverage associated with User
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5917EAC3-4DD6-4087-BFDE-146F61473141}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F89058B-BA23-4300-8411-22A2A7773C56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -128,7 +128,22 @@
   </si>
   <si>
     <t>Week 4ish: Getting passwords out of repo for Week 1 exercise
-Indie Project:  figuring out how to make sure cleandb.sql gets read during tests,  finishing most basic CRUD tests for UserDao, thinking about other methods to be built in dao, considering "todo" from week 4 about using equals instead of testing each property (no decision reached).</t>
+Indie Project:  figuring out how to make sure cleandb.sql gets read during tests,  finishing most basic CRUD tests for UserDao, thinking about other methods to be built in dao, considering "todo" from week 4 about using equals instead of testing each property (no decision reached).
+Week 5: started videos</t>
+  </si>
+  <si>
+    <t>Issues/Loose Ends:</t>
+  </si>
+  <si>
+    <t>// Instead of comparing all values
+        // it may make sense to use .equals()
+        // TODO review .equals recommendations http://docs.jboss.org/hibernate/orm/5.2/userguide/html_single/Hibernate_User_Guide.html#mapping-model-pojo-equalshashcode</t>
+  </si>
+  <si>
+    <t>I read the following but did not come to a conclusion about making a change in unit tests (did not change):</t>
+  </si>
+  <si>
+    <t>Mon9am</t>
   </si>
 </sst>
 </file>
@@ -496,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,34 +792,59 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43520</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
-        <v>26</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43521</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Annotates Story and Story/User association; fixes log4j2 properties to work with Windows
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BA3D20-8CD8-4619-9C1A-9928F7FBE6E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE44723-6A6E-4AA5-8E24-76677C906459}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="2340" yWindow="2415" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,13 +112,7 @@
 Indie Project: Prioritized User Stories and added tech suggestions to plans.</t>
   </si>
   <si>
-    <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose</t>
-  </si>
-  <si>
     <t>Indie Project: MVP ERD, populated lookup tables, tried to figure mysqldump (saved creation &amp; insert files separately for now), created User entity and draft dao, copied in SessionFactoryProvider</t>
-  </si>
-  <si>
-    <t>I have a log4j problem about renaming with the date etc, appears to be the same in week 1 exercise and project.</t>
   </si>
   <si>
     <t>Indie Project: setting up test database, properties, copying Database class, creating sql for cleaning database before testing, starting UserDaoTest, setting up log4j properties, changing mysql username and pw, trying to delete sensitive files from GitHub, troubleshooting why my cleandb.sql isn't actually running...</t>
@@ -143,11 +137,17 @@
     <t>I read the following but did not come to a conclusion about making a change in unit tests (did not change):</t>
   </si>
   <si>
-    <t>Mon9am - 10:30, 11 - 12, 1:30 - 2:20</t>
-  </si>
-  <si>
     <t>Week 4/Project: Completed Exercise 4 with javadocs and test results. Looked into question of what exactly session.save(object) returns.
 Week 5: Finished videos, reading (but would like to re-read the equals thing</t>
+  </si>
+  <si>
+    <t>Working on Log4J rolling files issue</t>
+  </si>
+  <si>
+    <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose… though adding a file name to the default location worked fine.</t>
+  </si>
+  <si>
+    <t>Resolved Log4J issue rolling files.</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +782,7 @@
         <v>6.5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>5.5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -804,28 +804,45 @@
         <v>3.5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43521</v>
       </c>
+      <c r="B28">
+        <v>3.5</v>
+      </c>
       <c r="D28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43522</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43524</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
@@ -833,29 +850,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="4:4" ht="75" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds StoryDao; Cleans up comments re: Story and User
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE44723-6A6E-4AA5-8E24-76677C906459}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F89A2-2292-41E1-8E8C-EDC28756EF3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2415" windowWidth="14640" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -147,14 +147,51 @@
     <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose… though adding a file name to the default location worked fine.</t>
   </si>
   <si>
-    <t>Resolved Log4J issue rolling files.</t>
+    <t>Resolved Log4J issue rolling files.  Feedback on presentation (yesterday).  Finished annotations for Story class and associating User and Story.  Generated basic functions for Story.</t>
+  </si>
+  <si>
+    <t>Fri 4:;45 - Setting up remaining methods for Story and User</t>
+  </si>
+  <si>
+    <t>// Finish Week 5 and Lookup Hibernate Search before digging in</t>
+  </si>
+  <si>
+    <t>Removed from UserDao comments -- save for a later time, differetn place</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>TODO get all users by number of removals or admin edits associated with their account</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>TODO get all users with income near the search criteria and the same family size</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +203,23 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,6 +253,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -515,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,46 +889,77 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43524</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="D41" s="2" t="s">
+    <row r="46" spans="4:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
StoryDaoTest passes 4 CRUD tests; getByPropertyNameSuccess() is started
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C97A8A-C522-4D39-A7D6-0AC2D9C07E25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6146F7-D7A9-4BC2-96AD-81BFAEEEDC18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -127,14 +127,6 @@
   </si>
   <si>
     <t>Issues/Loose Ends:</t>
-  </si>
-  <si>
-    <t>// Instead of comparing all values
-        // it may make sense to use .equals()
-        // TODO review .equals recommendations http://docs.jboss.org/hibernate/orm/5.2/userguide/html_single/Hibernate_User_Guide.html#mapping-model-pojo-equalshashcode</t>
-  </si>
-  <si>
-    <t>I read the following but did not come to a conclusion about making a change in unit tests (did not change):</t>
   </si>
   <si>
     <t>Week 4/Project: Completed Exercise 4 with javadocs and test results. Looked into question of what exactly session.save(object) returns.
@@ -184,16 +176,13 @@
     </r>
   </si>
   <si>
-    <t>Todo - test new methods in User; complete javadocs for user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.
-2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.
-2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.
-</t>
-  </si>
-  <si>
-    <t>Setting up and testing remaining methods for User.</t>
+    <t>Todo - complete javadocs for user; figure out where to test cascading deletes</t>
+  </si>
+  <si>
+    <t>Setting up and testing remaining methods for User, StoryDao testing, looking into date conversions (turned out to be unnecessary).</t>
+  </si>
+  <si>
+    <t>2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
   </si>
 </sst>
 </file>
@@ -254,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,7 +259,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +873,7 @@
         <v>3.5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -907,85 +895,75 @@
         <v>2.5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>47150</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43525</v>
       </c>
       <c r="B31">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D46" s="2" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="4:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="6"/>
+      <c r="D56" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replaces getByProperty with getByPropertyLike in StoryDao
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6146F7-D7A9-4BC2-96AD-81BFAEEEDC18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C22E51-C24B-40B1-98C4-5A98275C49B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -183,6 +183,16 @@
   </si>
   <si>
     <t>2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
+  </si>
+  <si>
+    <t>Indie Project: figuring out getByProperty issue in StoryDaoTest; reviewing generic dao examples
+Week 5: watched follow up videos</t>
+  </si>
+  <si>
+    <t>1+ hr 1st thing</t>
+  </si>
+  <si>
+    <t>7:05-x</t>
   </si>
 </sst>
 </file>
@@ -575,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +919,24 @@
         <v>42</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43526</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Improves UserDaoTest addWithProfileStory test, still passing
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C22E51-C24B-40B1-98C4-5A98275C49B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C10AFC0-0F46-44FF-918D-24EE8AA517C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -176,9 +176,6 @@
     </r>
   </si>
   <si>
-    <t>Todo - complete javadocs for user; figure out where to test cascading deletes</t>
-  </si>
-  <si>
     <t>Setting up and testing remaining methods for User, StoryDao testing, looking into date conversions (turned out to be unnecessary).</t>
   </si>
   <si>
@@ -193,6 +190,12 @@
   </si>
   <si>
     <t>7:05-x</t>
+  </si>
+  <si>
+    <t>Todo - complete javadocs for user; figure out where to test cascading deletes; complete javadocs for story; refactor tests to use .equals</t>
+  </si>
+  <si>
+    <t>TODO - Add unit tests to thoroughly test each method in your DAOs. Be sure that you are testing insert and delete of the associated records.</t>
   </si>
 </sst>
 </file>
@@ -583,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -924,74 +927,79 @@
         <v>43526</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="2" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
+    <row r="44" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+    <row r="46" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52"/>
-    </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="D53"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="6"/>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Successfully deletes user without deleting stories they only edited
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C10AFC0-0F46-44FF-918D-24EE8AA517C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDAFED0-6833-46AC-9830-0C5AF2F234D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -182,20 +182,14 @@
     <t>2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
   </si>
   <si>
-    <t>Indie Project: figuring out getByProperty issue in StoryDaoTest; reviewing generic dao examples
+    <t>Todo - complete javadocs for user; figure out where to test cascading deletes; complete javadocs for story; refactor tests to use .equals</t>
+  </si>
+  <si>
+    <t>TODO - Add unit tests to thoroughly test each method in your DAOs. Be sure that you are testing insert and delete of the associated records.</t>
+  </si>
+  <si>
+    <t>Indie Project: figuring out getByProperty issue in StoryDaoTest; reviewing generic dao examples; worked on testing effects of insert and delete on associated entities
 Week 5: watched follow up videos</t>
-  </si>
-  <si>
-    <t>1+ hr 1st thing</t>
-  </si>
-  <si>
-    <t>7:05-x</t>
-  </si>
-  <si>
-    <t>Todo - complete javadocs for user; figure out where to test cascading deletes; complete javadocs for story; refactor tests to use .equals</t>
-  </si>
-  <si>
-    <t>TODO - Add unit tests to thoroughly test each method in your DAOs. Be sure that you are testing insert and delete of the associated records.</t>
   </si>
 </sst>
 </file>
@@ -586,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="A34" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,84 +916,77 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43526</v>
       </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
       <c r="D32" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="s">
-        <v>46</v>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D46" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51"/>
+    </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
-        <v>38</v>
+      <c r="D52" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53"/>
+      <c r="D53" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="6"/>
+      <c r="D55" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds UserTest (4/4 tests passing)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDAFED0-6833-46AC-9830-0C5AF2F234D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B021AC8D-34F9-4F39-BC85-A0FEB84CCD97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Week 4: Worked on demo videos</t>
-  </si>
-  <si>
-    <t>NOT RESOLVED: getting correct path for mysqldump (don't need to do it yet so defering…)</t>
   </si>
   <si>
     <t>Week 4: Finished demo videos, Activity 1, and reading.
@@ -134,9 +131,6 @@
   </si>
   <si>
     <t>Working on Log4J rolling files issue</t>
-  </si>
-  <si>
-    <t>Now I have a path to get at mysqldump but I have an access problem for writing the dump to the locations I choose… though adding a file name to the default location worked fine.</t>
   </si>
   <si>
     <t>Resolved Log4J issue rolling files.  Feedback on presentation (yesterday).  Finished annotations for Story class and associating User and Story.  Generated basic functions for Story.</t>
@@ -185,11 +179,20 @@
     <t>Todo - complete javadocs for user; figure out where to test cascading deletes; complete javadocs for story; refactor tests to use .equals</t>
   </si>
   <si>
-    <t>TODO - Add unit tests to thoroughly test each method in your DAOs. Be sure that you are testing insert and delete of the associated records.</t>
-  </si>
-  <si>
     <t>Indie Project: figuring out getByProperty issue in StoryDaoTest; reviewing generic dao examples; worked on testing effects of insert and delete on associated entities
 Week 5: watched follow up videos</t>
+  </si>
+  <si>
+    <t>Useful mysql tutorial: used for changing foreign key constraint:</t>
+  </si>
+  <si>
+    <t>http://www.mysqltutorial.org/mysql-foreign-key/</t>
+  </si>
+  <si>
+    <t>PM - maybe 1 hour spread over many distractions?  Figuring out how to delete user without deleting their edited stories.</t>
+  </si>
+  <si>
+    <t>3pm - x</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +839,7 @@
         <v>5.5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -847,7 +850,7 @@
         <v>6.5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -858,7 +861,7 @@
         <v>5.5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -869,7 +872,7 @@
         <v>3.5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -880,7 +883,7 @@
         <v>3.5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -902,7 +905,7 @@
         <v>2.5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -913,7 +916,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -924,47 +927,42 @@
         <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
@@ -972,21 +970,31 @@
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="6"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds draft controller and logic shells
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E51713-9CA6-4072-BEA3-0CC1B7ECE2D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9052F35A-979F-4C58-BF18-E86E7FCB8523}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -199,7 +199,11 @@
   </si>
   <si>
     <t>Verified no PW's in unexpected places
-Week 6: submitted professional dev feedback, installed Putty, worked through the rest of AWS exercise</t>
+Week 6: submitted professional dev feedback, installed Putty, worked through the rest of AWS exercise videos but left off on actual exercise at the point of getting database set up (step 5).  Hoping to do step 6 after more project work is complete.</t>
+  </si>
+  <si>
+    <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells
+Week 7: Intro video</t>
   </si>
 </sst>
 </file>
@@ -260,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -274,6 +278,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -590,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,81 +966,90 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43529</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43530</v>
+      </c>
+      <c r="B36">
+        <v>3.5</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="s">
+      <c r="D37" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="2" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="s">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50"/>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="5" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="5" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="5" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="6"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="6"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds basic unmapped entities for existing tables except story_removals (which I might change)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9052F35A-979F-4C58-BF18-E86E7FCB8523}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BC4B5E-7CCF-418E-8FD9-9EE8A0E47FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -202,7 +202,10 @@
 Week 6: submitted professional dev feedback, installed Putty, worked through the rest of AWS exercise videos but left off on actual exercise at the point of getting database set up (step 5).  Hoping to do step 6 after more project work is complete.</t>
   </si>
   <si>
-    <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells
+    <t>TODO - consider different approach for recording story removals -- I have a bad hunch about current approach</t>
+  </si>
+  <si>
+    <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells and super basic entity classes
 Week 7: Intro video</t>
   </si>
 </sst>
@@ -599,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,15 +985,20 @@
         <v>43530</v>
       </c>
       <c r="B36">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">

</xml_diff>

<commit_message>
Refines TODOs for search logic class
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BC4B5E-7CCF-418E-8FD9-9EE8A0E47FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F483A4A-BA5C-4591-9867-58A174DA3E61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -207,6 +207,12 @@
   <si>
     <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells and super basic entity classes
 Week 7: Intro video</t>
+  </si>
+  <si>
+    <t>Indi Project: consider how logic class will work - is it really a special dao?</t>
+  </si>
+  <si>
+    <t>Thurs 5 am - ?</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,72 +998,89 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="1">
+        <v>43531</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="s">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="D39" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+    <row r="51" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54"/>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="5" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="5" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="6"/>
-    </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="6"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="2" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drafts generic dao, checked against existing daos for content
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F483A4A-BA5C-4591-9867-58A174DA3E61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1927AF-0866-4F16-B8BE-77EAD9882424}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -209,10 +209,10 @@
 Week 7: Intro video</t>
   </si>
   <si>
-    <t>Indi Project: consider how logic class will work - is it really a special dao?</t>
-  </si>
-  <si>
-    <t>Thurs 5 am - ?</t>
+    <t>Thurs 5 am - 6:45</t>
+  </si>
+  <si>
+    <t>Indi Project: consider how logic class will work - is it really a special dao?; Drafted generic dao</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,7 +1002,7 @@
         <v>43531</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="D39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Accommodates new database features in cleandb.sql; removes outdated sql dumps
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1927AF-0866-4F16-B8BE-77EAD9882424}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7B463-4F85-4618-B4AB-821A3BE2ADB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -212,7 +212,10 @@
     <t>Thurs 5 am - 6:45</t>
   </si>
   <si>
-    <t>Indi Project: consider how logic class will work - is it really a special dao?; Drafted generic dao</t>
+    <t>Indie Project: consider how logic class will work - is it really a special dao?; Drafted generic dao</t>
+  </si>
+  <si>
+    <t>11:45 - x</t>
   </si>
 </sst>
 </file>
@@ -606,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,71 +1019,83 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="D40" s="7"/>
+      <c r="D40" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="2" t="s">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
+    <row r="54" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="5" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="5" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="6"/>
-    </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="6"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Organizes initial files in webapp
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7B463-4F85-4618-B4AB-821A3BE2ADB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A52E6-F76C-430A-84F8-4FC4E859F17B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -136,38 +136,7 @@
     <t>Resolved Log4J issue rolling files.  Feedback on presentation (yesterday).  Finished annotations for Story class and associating User and Story.  Generated basic functions for Story.</t>
   </si>
   <si>
-    <t>// Finish Week 5 and Lookup Hibernate Search before digging in</t>
-  </si>
-  <si>
     <t>Removed from UserDao comments -- save for a later time, differetn place</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">// </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>TODO get all users by number of removals or admin edits associated with their account</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">// </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>TODO get all users with income near the search criteria and the same family size</t>
-    </r>
   </si>
   <si>
     <t>Setting up and testing remaining methods for User, StoryDao testing, looking into date conversions (turned out to be unnecessary).</t>
@@ -186,12 +155,6 @@
 Week 5: watched follow up videos</t>
   </si>
   <si>
-    <t>Todo -  refactor tests to use .equals when I go back and make a generic dao</t>
-  </si>
-  <si>
-    <t>double check that I'm not getting passwords back into github with the idea data files</t>
-  </si>
-  <si>
     <t>Week 6: Intro video, AWS account setup, starting to read</t>
   </si>
   <si>
@@ -202,27 +165,30 @@
 Week 6: submitted professional dev feedback, installed Putty, worked through the rest of AWS exercise videos but left off on actual exercise at the point of getting database set up (step 5).  Hoping to do step 6 after more project work is complete.</t>
   </si>
   <si>
-    <t>TODO - consider different approach for recording story removals -- I have a bad hunch about current approach</t>
-  </si>
-  <si>
     <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells and super basic entity classes
 Week 7: Intro video</t>
   </si>
   <si>
-    <t>Thurs 5 am - 6:45</t>
-  </si>
-  <si>
-    <t>Indie Project: consider how logic class will work - is it really a special dao?; Drafted generic dao</t>
-  </si>
-  <si>
-    <t>11:45 - x</t>
+    <t>TODO (nice to do)  -  refactor tests to use .equals in UserDaoTest and StoryDaoTest</t>
+  </si>
+  <si>
+    <t>^^^ Recently unable to re-create</t>
+  </si>
+  <si>
+    <t>TODO NEXT - figure out how to set up web.xml… use old project as model?  Or exercise 1?  Is maven supposed to help make this - I don't remember!!</t>
+  </si>
+  <si>
+    <t>Indie Project: consider how logic class will work - is it really a special dao?; revised database design and associated classes; implemented GenericDao, started a profile JSP</t>
+  </si>
+  <si>
+    <t>OOOOSPS starter web-app is in the project already… I totally don't remember how to get it to launch.  Is some kind of setup needed that I am missing from this project?  Also need to get rid of my extra web-app folder and put stuff where it belongs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,23 +200,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,12 +233,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -609,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -953,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -986,7 +929,7 @@
         <v>4.5</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -997,15 +940,18 @@
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43531</v>
       </c>
+      <c r="B37">
+        <v>4.5</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1013,90 +959,64 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="D39" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="D40" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+      <c r="D41" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
-        <v>44</v>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60"/>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="6"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
-        <v>42</v>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Develops ExperiencesSearch further and starts a query list (ListOfQuestions)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A52E6-F76C-430A-84F8-4FC4E859F17B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEF0D47-16E3-4F2E-990A-6A2D7B049D61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -175,13 +175,17 @@
     <t>^^^ Recently unable to re-create</t>
   </si>
   <si>
-    <t>TODO NEXT - figure out how to set up web.xml… use old project as model?  Or exercise 1?  Is maven supposed to help make this - I don't remember!!</t>
-  </si>
-  <si>
     <t>Indie Project: consider how logic class will work - is it really a special dao?; revised database design and associated classes; implemented GenericDao, started a profile JSP</t>
   </si>
   <si>
-    <t>OOOOSPS starter web-app is in the project already… I totally don't remember how to get it to launch.  Is some kind of setup needed that I am missing from this project?  Also need to get rid of my extra web-app folder and put stuff where it belongs.</t>
+    <t xml:space="preserve">Indie Project: organized webapp and set up run config in IntelliJ. Added some data to "production" db.  Got profile.jsp to display username from db.  </t>
+  </si>
+  <si>
+    <t>6:45 - x</t>
+  </si>
+  <si>
+    <t>Indi Project: exploring how hibernate queries work with associated tables, developing ExperiencesSearch and list of questions to help complete UML diagram
+Week 6:</t>
   </si>
 </sst>
 </file>
@@ -552,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,71 +955,87 @@
         <v>4.5</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43533</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43534</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="D40" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="D41" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="49" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53"/>
-    </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="2" t="s">
+      <c r="D55"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates Project Plan; Drafts UML Diagram
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEF0D47-16E3-4F2E-990A-6A2D7B049D61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCFA90C-62F5-44B2-80BA-1D79CF323AEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -181,11 +181,11 @@
     <t xml:space="preserve">Indie Project: organized webapp and set up run config in IntelliJ. Added some data to "production" db.  Got profile.jsp to display username from db.  </t>
   </si>
   <si>
-    <t>6:45 - x</t>
-  </si>
-  <si>
     <t>Indi Project: exploring how hibernate queries work with associated tables, developing ExperiencesSearch and list of questions to help complete UML diagram
 Week 6:</t>
+  </si>
+  <si>
+    <t>Indie Project/Week 6: worked out issues concerning access to AWS EC2 instance.  Project is now deployed and public, and SSH works from classroom.</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,21 +973,29 @@
       <c r="A39" s="1">
         <v>43534</v>
       </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
       <c r="D39" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43535</v>
+      </c>
+      <c r="B40">
+        <v>1.5</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="D42" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>

</xml_diff>

<commit_message>
Adds capability to search using multiple criteria (dao) and to display a story on the profile
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCFA90C-62F5-44B2-80BA-1D79CF323AEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8C34C6-76B9-4515-8C8C-332F3AFEC8E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Indie Project/Week 6: worked out issues concerning access to AWS EC2 instance.  Project is now deployed and public, and SSH works from classroom.</t>
+  </si>
+  <si>
+    <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp.</t>
   </si>
 </sst>
 </file>
@@ -556,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,8 +994,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43536</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -1002,48 +1013,54 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
+    <row r="51" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55"/>
-    </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+      <c r="D57"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reverses 1:1 directionality with Survey and starts annotations
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8C34C6-76B9-4515-8C8C-332F3AFEC8E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51351BA-14C2-4392-B5FB-D306A5A67798}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -188,7 +188,10 @@
     <t>Indie Project/Week 6: worked out issues concerning access to AWS EC2 instance.  Project is now deployed and public, and SSH works from classroom.</t>
   </si>
   <si>
-    <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp.</t>
+    <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.</t>
+  </si>
+  <si>
+    <t>plus9:55 - 11:40</t>
   </si>
 </sst>
 </file>
@@ -561,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,12 +997,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43536</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>51</v>
@@ -1013,6 +1016,9 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
+      <c r="D44" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>

</xml_diff>

<commit_message>
Drafts hibernate annotations for lookup tables (untested, no add/remove methods for survey sets)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51351BA-14C2-4392-B5FB-D306A5A67798}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F98CA-9360-4658-B5E1-DB3279F24497}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -191,7 +191,10 @@
     <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.</t>
   </si>
   <si>
-    <t>plus9:55 - 11:40</t>
+    <t>plus9:55 - 12:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plus 12:20 - </t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1025,9 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
+      <c r="D45" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>

</xml_diff>

<commit_message>
Updates cleandb and adds Survey Dao Tests (5/5 pass)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F98CA-9360-4658-B5E1-DB3279F24497}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFFA99A-F89A-472C-A71F-EEB928305681}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -188,13 +188,10 @@
     <t>Indie Project/Week 6: worked out issues concerning access to AWS EC2 instance.  Project is now deployed and public, and SSH works from classroom.</t>
   </si>
   <si>
-    <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.</t>
-  </si>
-  <si>
-    <t>plus9:55 - 12:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plus 12:20 - </t>
+    <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.  Testing and troubleshooting.</t>
+  </si>
+  <si>
+    <t>Thurs 8:50 - x</t>
   </si>
 </sst>
 </file>
@@ -567,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,14 +1002,16 @@
         <v>43536</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1">
+        <v>43538</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -1025,9 +1024,6 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="D45" s="2" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>

</xml_diff>

<commit_message>
Makes database conform to authentication requirements for role and user. (Entities not yet updated)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFFA99A-F89A-472C-A71F-EEB928305681}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30FDFC3-E866-4985-8B48-16C14CDDDB5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -191,7 +191,10 @@
     <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.  Testing and troubleshooting.</t>
   </si>
   <si>
-    <t>Thurs 8:50 - x</t>
+    <t>Indie Project: Brought Survey Dao Tests to 5/5 passing; Noted programming decisions that are needed for searching surveys.</t>
+  </si>
+  <si>
+    <t>Thurs 8:50 - 10:30, 11:15-x</t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1015,9 @@
       <c r="A42" s="1">
         <v>43538</v>
       </c>
+      <c r="D42" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -1019,7 +1025,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="D44" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1027,48 +1033,57 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
+    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57"/>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="2" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drafts changes needed for authentication
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30FDFC3-E866-4985-8B48-16C14CDDDB5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9D9962-4069-48CA-8564-BDE418D2639E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -191,10 +191,11 @@
     <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.  Testing and troubleshooting.</t>
   </si>
   <si>
-    <t>Indie Project: Brought Survey Dao Tests to 5/5 passing; Noted programming decisions that are needed for searching surveys.</t>
-  </si>
-  <si>
-    <t>Thurs 8:50 - 10:30, 11:15-x</t>
+    <t>Thurs -  a little more time than listed.</t>
+  </si>
+  <si>
+    <t>Indie Project: Brought Survey Dao Tests to 5/5 passing; Noted programming decisions that are needed for searching surveys.  Revised tables (and other files as needed) to structure the roles table as neede for authentication.  Created data for the application database.
+Week 7: Started videos, following along in project.</t>
   </si>
 </sst>
 </file>
@@ -568,7 +569,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD48"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,12 +1012,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43538</v>
       </c>
+      <c r="B42">
+        <v>6.5</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,7 +1029,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="D44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Displays profile, without story header, if there is no financial story.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9D9962-4069-48CA-8564-BDE418D2639E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B393DE-CE7B-4A8A-8CF3-7AF60B92C745}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -196,6 +196,9 @@
   <si>
     <t>Indie Project: Brought Survey Dao Tests to 5/5 passing; Noted programming decisions that are needed for searching surveys.  Revised tables (and other files as needed) to structure the roles table as neede for authentication.  Created data for the application database.
 Week 7: Started videos, following along in project.</t>
+  </si>
+  <si>
+    <t>Week 7/Project: worked on web.xml changes and package changes for authentication.</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,13 +1027,18 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1">
+        <v>43539</v>
+      </c>
+      <c r="B43">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="D44" s="2" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -1040,54 +1048,66 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
+      <c r="D47" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="2" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds separate error displays for 403's and other errors. Authentication works in local dev environment.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B393DE-CE7B-4A8A-8CF3-7AF60B92C745}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF9B0FA-B5F1-4BC4-91BE-23F1AE977E6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>Week 7/Project: worked on web.xml changes and package changes for authentication.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO WEEK 7 - • TODO google “web xml custom error pages” and implement
+• Maybe this one https://www.tutorialspoint.com/servlets/servlets-exception-handling.htm
+</t>
+  </si>
+  <si>
+    <t>Week 7: Completed readings (light treatment) and videos
+Indie Project: added separate jsp's for 403 errors and other errors</t>
   </si>
 </sst>
 </file>
@@ -569,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,14 +1040,22 @@
         <v>43539</v>
       </c>
       <c r="B43">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43540</v>
+      </c>
+      <c r="B44">
+        <v>2.5</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -1048,12 +1065,12 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="D47" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
+      <c r="D48" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -1063,51 +1080,66 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
+      <c r="D51" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="2" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sets up some info for Hibernate Search (no function); authentication works.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF9B0FA-B5F1-4BC4-91BE-23F1AE977E6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306BC62B-B6BE-48B6-82AA-5D0806F78D53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Indie Project: Trying Paula's example function for retrieving an entity based on its own characteristics and that of another entity. Tested it in StoryDaoTest. Used it for the profile display servlet/jsp. Added hibernate assocations for survey tables; reviewed 1:1 relationships. changed DB FK directionality for 1:1 relationships with survey.  Testing and troubleshooting.</t>
   </si>
   <si>
-    <t>Thurs -  a little more time than listed.</t>
-  </si>
-  <si>
     <t>Indie Project: Brought Survey Dao Tests to 5/5 passing; Noted programming decisions that are needed for searching surveys.  Revised tables (and other files as needed) to structure the roles table as neede for authentication.  Created data for the application database.
 Week 7: Started videos, following along in project.</t>
   </si>
@@ -201,13 +198,18 @@
     <t>Week 7/Project: worked on web.xml changes and package changes for authentication.</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO WEEK 7 - • TODO google “web xml custom error pages” and implement
-• Maybe this one https://www.tutorialspoint.com/servlets/servlets-exception-handling.htm
-</t>
-  </si>
-  <si>
-    <t>Week 7: Completed readings (light treatment) and videos
-Indie Project: added separate jsp's for 403 errors and other errors</t>
+    <t>Week 7: Completed readings (light treatment) and videos; added hibernate search to pom, made cfg changes, added annotations
+Indie Project: added separate jsp's for 403 errors and other errors
+Professional Development: Researching Hibernate Search; started a ppt</t>
+  </si>
+  <si>
+    <t>Indie Project: trying to figure out how to create index from existing database for Hibernate Search.  Troubleshooting NPE that I swear wasn't there before.</t>
+  </si>
+  <si>
+    <t>Eliminated the NPE!!!</t>
+  </si>
+  <si>
+    <t>Friday 9pm - x…</t>
   </si>
 </sst>
 </file>
@@ -251,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -259,9 +261,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -578,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1031,7 @@
         <v>6.5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,33 +1042,49 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43540</v>
       </c>
       <c r="B44">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43541</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43546</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="D48" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,68 +1093,46 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="D53" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D61" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67"/>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uses authentication for accessing profile and admin pages via servlet. May meet minimal week 7 requirements.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306BC62B-B6BE-48B6-82AA-5D0806F78D53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6BD79B-56B7-4EC5-8E21-9528C656F4E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -206,10 +206,8 @@
     <t>Indie Project: trying to figure out how to create index from existing database for Hibernate Search.  Troubleshooting NPE that I swear wasn't there before.</t>
   </si>
   <si>
-    <t>Eliminated the NPE!!!</t>
-  </si>
-  <si>
-    <t>Friday 9pm - x…</t>
+    <t>Indie Project: Eliminated the NPE!!!
+Week 7/Indie Project: drafted servlet and jsp for admin to use, to demo authentication.  Not working yet, probably due to path issues.</t>
   </si>
 </sst>
 </file>
@@ -577,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="A48" sqref="A48:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,12 +1065,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43546</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>56</v>
@@ -1081,58 +1079,46 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempts a hibernate search in SearchExperiences. No success yet.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6BD79B-56B7-4EC5-8E21-9528C656F4E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A07DD46-F9B5-4878-A9CF-92179ED97D23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -208,6 +208,10 @@
   <si>
     <t>Indie Project: Eliminated the NPE!!!
 Week 7/Indie Project: drafted servlet and jsp for admin to use, to demo authentication.  Not working yet, probably due to path issues.</t>
+  </si>
+  <si>
+    <t>Week 7: got authentication working for admin and profile pages.  Tried to stop direct access via jsp but that didn't seem to work.
+Fixed config so it doesn't kill my program.  Attempted a hibernate search - not getting expected result yet.</t>
   </si>
 </sst>
 </file>
@@ -575,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD50"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,49 +1080,69 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43547</v>
+      </c>
+      <c r="B47">
+        <v>7.5</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
+    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="2" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58"/>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="2" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="2" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Succeeds in executing a simple Hibernate Search
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A07DD46-F9B5-4878-A9CF-92179ED97D23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE0A3DA-A3A5-46F0-BB7F-4010B4771B7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>Week 7: got authentication working for admin and profile pages.  Tried to stop direct access via jsp but that didn't seem to work.
 Fixed config so it doesn't kill my program.  Attempted a hibernate search - not getting expected result yet.</t>
+  </si>
+  <si>
+    <t>TODO -- PW feedback week 7: No deal breakers there. You might consider toggling the log-in button to "log out" if   a user is already logged in.  Log out should trigger a session.invalidate() type method to removed the logged in user's info from session. Hope that helps!</t>
+  </si>
+  <si>
+    <t>TODO-- Week 7 see PW snippet for better servlet mapping</t>
   </si>
 </sst>
 </file>
@@ -581,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,11 +1100,17 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
+      <c r="D49" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
+      <c r="D50" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>

</xml_diff>

<commit_message>
Maybe adds comments?  Last commit before attempting fuzzy search
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE0A3DA-A3A5-46F0-BB7F-4010B4771B7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEE7346-19E8-4B2A-9D10-519BF4DC32A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>TODO-- Week 7 see PW snippet for better servlet mapping</t>
+  </si>
+  <si>
+    <t>Project/Presentation: Got code working to backfill the indexes for Hibernate Search; completed a successful search; worked on PowerPoint</t>
+  </si>
+  <si>
+    <t>2.5 doucmented plus Sun 10:10 - 11:45</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -269,6 +275,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -585,9 +594,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1097,64 +1106,93 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43548</v>
+      </c>
+      <c r="B48">
+        <v>2.5</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="D49" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="D55" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="D56" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
+    <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
+    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleans up comments in SearchExperiences servlet
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEE7346-19E8-4B2A-9D10-519BF4DC32A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C131956-059D-4C94-BC45-84F073D3CCB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2460" windowWidth="14925" windowHeight="13140" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -220,10 +220,7 @@
     <t>TODO-- Week 7 see PW snippet for better servlet mapping</t>
   </si>
   <si>
-    <t>Project/Presentation: Got code working to backfill the indexes for Hibernate Search; completed a successful search; worked on PowerPoint</t>
-  </si>
-  <si>
-    <t>2.5 doucmented plus Sun 10:10 - 11:45</t>
+    <t>Project/Presentation: Got code working to backfill the indexes for Hibernate Search; completed several kinds of searchs; completed presentation materials</t>
   </si>
 </sst>
 </file>
@@ -596,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1108,7 @@
         <v>43548</v>
       </c>
       <c r="B48">
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>60</v>
@@ -1122,9 +1119,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="D50" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>

</xml_diff>

<commit_message>
Adds header with nav and tagline
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C131956-059D-4C94-BC45-84F073D3CCB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387E4D85-9078-491F-9005-23C65A96A875}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -221,6 +221,16 @@
   </si>
   <si>
     <t>Project/Presentation: Got code working to backfill the indexes for Hibernate Search; completed several kinds of searchs; completed presentation materials</t>
+  </si>
+  <si>
+    <t>Week 8 overview video and reading</t>
+  </si>
+  <si>
+    <t>Week 8 Activities (including time spent sorting out how to handle file permissions in jdk lib)</t>
+  </si>
+  <si>
+    <t>Week 8 Activities (last things)
+Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.</t>
   </si>
 </sst>
 </file>
@@ -591,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,14 +1125,37 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="1">
+        <v>43549</v>
+      </c>
+      <c r="B49">
+        <v>1.5</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A50" s="1">
+        <v>43550</v>
+      </c>
+      <c r="B50">
+        <v>5.5</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43552</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -1133,61 +1166,73 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="D55" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="D56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="D59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="D60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
+    <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="2" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D62" s="2" t="s">
+    <row r="66" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68"/>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates DisplayProfile.java to display information for logged in user.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387E4D85-9078-491F-9005-23C65A96A875}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFCE520-85B5-4FFA-A1DE-76B921DE455B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -231,6 +231,30 @@
   <si>
     <t>Week 8 Activities (last things)
 Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.</t>
+  </si>
+  <si>
+    <t>THURS: above +1, 1 pm - x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday plan: </t>
+  </si>
+  <si>
+    <t>go through website and clean up any temporary links or anonymous and hard coded stuff</t>
+  </si>
+  <si>
+    <t>incorporate as much feedback as possible so far</t>
+  </si>
+  <si>
+    <t>deploy to aws to make sure hibernate search doesn't break</t>
+  </si>
+  <si>
+    <t>take an aws snapshot</t>
+  </si>
+  <si>
+    <t>check aws cost structure situation</t>
+  </si>
+  <si>
+    <t>TODO-- PW feedback authentication You may find that to get very fine-grained control over specific data when using a servlet that serve a couple different user types (view my profile versus view somebody else's profile), you may want to check the role within the servlet. The other option would be to set up two servlets ViewMyProfile versus ViewOtherProfile. I can think of pros and cons to each approach...</t>
   </si>
 </sst>
 </file>
@@ -601,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,77 +1186,119 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
+      <c r="D53" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
+      <c r="D55" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
+      <c r="D56" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
+      <c r="D57" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="D60" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="D64" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="D65" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="D66" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="2" t="s">
+    <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D66" s="2" t="s">
+    <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="2" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="2" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72"/>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="2" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starts testing retrieval of survey by user and starts putting profile pieces into place. Removes template with security issue.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFCE520-85B5-4FFA-A1DE-76B921DE455B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA697A-45CB-4473-851D-904B11F41AB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -229,32 +229,32 @@
     <t>Week 8 Activities (including time spent sorting out how to handle file permissions in jdk lib)</t>
   </si>
   <si>
+    <t>THURS: above +1, 1 pm - x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday plan: </t>
+  </si>
+  <si>
+    <t>go through website and clean up any temporary links or anonymous and hard coded stuff</t>
+  </si>
+  <si>
+    <t>incorporate as much feedback as possible so far</t>
+  </si>
+  <si>
+    <t>deploy to aws to make sure hibernate search doesn't break</t>
+  </si>
+  <si>
+    <t>take an aws snapshot</t>
+  </si>
+  <si>
+    <t>check aws cost structure situation</t>
+  </si>
+  <si>
+    <t>TODO-- PW feedback authentication You may find that to get very fine-grained control over specific data when using a servlet that serve a couple different user types (view my profile versus view somebody else's profile), you may want to check the role within the servlet. The other option would be to set up two servlets ViewMyProfile versus ViewOtherProfile. I can think of pros and cons to each approach...</t>
+  </si>
+  <si>
     <t>Week 8 Activities (last things)
-Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.</t>
-  </si>
-  <si>
-    <t>THURS: above +1, 1 pm - x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thursday plan: </t>
-  </si>
-  <si>
-    <t>go through website and clean up any temporary links or anonymous and hard coded stuff</t>
-  </si>
-  <si>
-    <t>incorporate as much feedback as possible so far</t>
-  </si>
-  <si>
-    <t>deploy to aws to make sure hibernate search doesn't break</t>
-  </si>
-  <si>
-    <t>take an aws snapshot</t>
-  </si>
-  <si>
-    <t>check aws cost structure situation</t>
-  </si>
-  <si>
-    <t>TODO-- PW feedback authentication You may find that to get very fine-grained control over specific data when using a servlet that serve a couple different user types (view my profile versus view somebody else's profile), you may want to check the role within the servlet. The other option would be to set up two servlets ViewMyProfile versus ViewOtherProfile. I can think of pros and cons to each approach...</t>
+Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.  Added header jsp and got rid of random links in jsps.  Developed search jsps and servlets that connect to each other (don't properly handle info yet).  Working on profile jsp and servlet.  working on SurveyDaoTest as part of that.</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,15 +1170,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43552</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="D53" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,37 +1196,37 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="D55" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="D56" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="D57" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="D60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
     <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Successfully tests retrieval of a user's survey, assuming only 1. Displays partial survey data in profile.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA697A-45CB-4473-851D-904B11F41AB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80484A2B-3BB0-4B42-9087-B17E0E99819A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Week 8 Activities (including time spent sorting out how to handle file permissions in jdk lib)</t>
-  </si>
-  <si>
-    <t>THURS: above +1, 1 pm - x</t>
   </si>
   <si>
     <t xml:space="preserve">Thursday plan: </t>
@@ -627,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1175,7 @@
         <v>6.5</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,9 +1183,6 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="D53" s="2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
@@ -1196,37 +1190,37 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="D55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="D56" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="D57" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="D60" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,7 +1235,7 @@
     <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improves JSP/servlet interaction for stats search. Breaks SearchExperiences.java - messes up the request URI somehow.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80484A2B-3BB0-4B42-9087-B17E0E99819A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47019702-AE6D-4849-86A9-A4564A087CFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -252,6 +252,12 @@
   <si>
     <t>Week 8 Activities (last things)
 Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.  Added header jsp and got rid of random links in jsps.  Developed search jsps and servlets that connect to each other (don't properly handle info yet).  Working on profile jsp and servlet.  working on SurveyDaoTest as part of that.</t>
+  </si>
+  <si>
+    <t>1-ish??</t>
+  </si>
+  <si>
+    <t>Cleaning up JSP/Servlet connections… or trying to anyway</t>
   </si>
 </sst>
 </file>
@@ -624,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1185,15 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1">
+        <v>43553</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>

</xml_diff>

<commit_message>
Resolves search issue by restricting search.jsp. Stops user from logging in while attempting search, which was what messed things up before.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47019702-AE6D-4849-86A9-A4564A087CFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8BF141-3490-4D78-B9D6-C07C674765FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>Cleaning up JSP/Servlet connections… or trying to anyway</t>
+  </si>
+  <si>
+    <t>Note:  I may have needed to do something in web xml to get my application startup servlet to actually load on startup</t>
+  </si>
+  <si>
+    <t>http://tutorials.jenkov.com/java-servlets/web-xml.html</t>
   </si>
 </sst>
 </file>
@@ -628,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,109 +1210,124 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="D55" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="D56" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="D57" s="2" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="D60" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
+      <c r="D61" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
+      <c r="D62" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="D64" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="D65" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="D66" s="2" t="s">
+    </row>
+    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="D67" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="D68" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="D69" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+    <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D80" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="2" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Displays (ugly) search-by-topic results. Not a fuzzy search yet.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8BF141-3490-4D78-B9D6-C07C674765FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D9EC1B-559B-49F8-B6F5-456393BE5B70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Enables user to log out. Gets rid of login nav item b/c causing problem. (replace in future?)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D9EC1B-559B-49F8-B6F5-456393BE5B70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6482AA38-BFC1-49DC-AC6E-5EDA10A99B2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -214,9 +214,6 @@
 Fixed config so it doesn't kill my program.  Attempted a hibernate search - not getting expected result yet.</t>
   </si>
   <si>
-    <t>TODO -- PW feedback week 7: No deal breakers there. You might consider toggling the log-in button to "log out" if   a user is already logged in.  Log out should trigger a session.invalidate() type method to removed the logged in user's info from session. Hope that helps!</t>
-  </si>
-  <si>
     <t>TODO-- Week 7 see PW snippet for better servlet mapping</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">Thursday plan: </t>
-  </si>
-  <si>
-    <t>go through website and clean up any temporary links or anonymous and hard coded stuff</t>
   </si>
   <si>
     <t>incorporate as much feedback as possible so far</t>
@@ -254,16 +248,19 @@
 Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.  Added header jsp and got rid of random links in jsps.  Developed search jsps and servlets that connect to each other (don't properly handle info yet).  Working on profile jsp and servlet.  working on SurveyDaoTest as part of that.</t>
   </si>
   <si>
-    <t>1-ish??</t>
-  </si>
-  <si>
-    <t>Cleaning up JSP/Servlet connections… or trying to anyway</t>
-  </si>
-  <si>
     <t>Note:  I may have needed to do something in web xml to get my application startup servlet to actually load on startup</t>
   </si>
   <si>
     <t>http://tutorials.jenkov.com/java-servlets/web-xml.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uh-oh, survey not mapped right or servlet doesn't display right: </t>
+  </si>
+  <si>
+    <t>Impact of other financial factors: Unmet goals caused frustration.</t>
+  </si>
+  <si>
+    <t>Indie Project: Cleaning up JSP/Servlet connections, getting rid of hard-coded search stuff, enabling log out.</t>
   </si>
 </sst>
 </file>
@@ -634,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,7 +1162,7 @@
         <v>1.5</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,7 +1173,7 @@
         <v>5.5</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1187,18 +1184,18 @@
         <v>6.5</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43553</v>
       </c>
-      <c r="B52" t="s">
-        <v>71</v>
+      <c r="B52">
+        <v>3.5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,18 +1203,18 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
+      <c r="D54" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="D55" s="2" t="s">
-        <v>73</v>
+      <c r="D55" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="D56" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -1225,32 +1222,26 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="D60" s="2" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="D61" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="D62" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
@@ -1260,74 +1251,89 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
+      <c r="D64" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
+      <c r="D65" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="D67" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="D68" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="D69" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+      <c r="D70" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="D72" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="2" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81"/>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="2" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes IncomeSkew mapping and tests retrieval of skew, needs, and goals descriptions by survey id (passes)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6482AA38-BFC1-49DC-AC6E-5EDA10A99B2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54B951E-6E35-4D9B-9F3B-4D32771732CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adds correctly functioning login to nav
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54B951E-6E35-4D9B-9F3B-4D32771732CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DB580C-99C0-4D0E-A261-EF48FC63D886}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -254,13 +254,10 @@
     <t>http://tutorials.jenkov.com/java-servlets/web-xml.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Uh-oh, survey not mapped right or servlet doesn't display right: </t>
-  </si>
-  <si>
-    <t>Impact of other financial factors: Unmet goals caused frustration.</t>
-  </si>
-  <si>
     <t>Indie Project: Cleaning up JSP/Servlet connections, getting rid of hard-coded search stuff, enabling log out.</t>
+  </si>
+  <si>
+    <t>Indie Project: Fixed IncomeSkew mapping, added new test for surveys to check details explicitly.  Added login servlet so I could reinstate the login nav option.</t>
   </si>
 </sst>
 </file>
@@ -633,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,23 +1192,22 @@
         <v>3.5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43554</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="D54" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="D55" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>

</xml_diff>

<commit_message>
Adds comments pertaining to using BLS API
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DB580C-99C0-4D0E-A261-EF48FC63D886}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288EA2B5-9DFA-4E76-8A7A-E91B25945982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -226,21 +226,6 @@
     <t>Week 8 Activities (including time spent sorting out how to handle file permissions in jdk lib)</t>
   </si>
   <si>
-    <t xml:space="preserve">Thursday plan: </t>
-  </si>
-  <si>
-    <t>incorporate as much feedback as possible so far</t>
-  </si>
-  <si>
-    <t>deploy to aws to make sure hibernate search doesn't break</t>
-  </si>
-  <si>
-    <t>take an aws snapshot</t>
-  </si>
-  <si>
-    <t>check aws cost structure situation</t>
-  </si>
-  <si>
     <t>TODO-- PW feedback authentication You may find that to get very fine-grained control over specific data when using a servlet that serve a couple different user types (view my profile versus view somebody else's profile), you may want to check the role within the servlet. The other option would be to set up two servlets ViewMyProfile versus ViewOtherProfile. I can think of pros and cons to each approach...</t>
   </si>
   <si>
@@ -257,7 +242,23 @@
     <t>Indie Project: Cleaning up JSP/Servlet connections, getting rid of hard-coded search stuff, enabling log out.</t>
   </si>
   <si>
-    <t>Indie Project: Fixed IncomeSkew mapping, added new test for surveys to check details explicitly.  Added login servlet so I could reinstate the login nav option.</t>
+    <t>Indie Project: Fixed IncomeSkew mapping, added new test for surveys to check details explicitly.  Added login servlet so I could reinstate the login nav option. Trouble-shot why amazon deploy didn't work - fixed it.  Checkpoint 3 done!</t>
+  </si>
+  <si>
+    <t>Week 9: Videos through activity 1
+Indie Project: got BLS api key and figured out which kind of survey/series ID I think I'll use</t>
+  </si>
+  <si>
+    <t>Week 9: Remaining videos + a couple readings, professional dev feedback</t>
+  </si>
+  <si>
+    <t>^^^ Doesn't that servlet mapping still allow JSP's to accessed directly? Do I need to do the mapping?</t>
+  </si>
+  <si>
+    <t>Week 9: Activities - finished activities (with question) but not exercise.  See PW answer re: JSON, probably apply in Exercise rather than in activity.</t>
+  </si>
+  <si>
+    <t>Sun 11 - x Review activity 4 &amp; kelly's work</t>
   </si>
 </sst>
 </file>
@@ -628,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1182,7 @@
         <v>6.5</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,25 +1193,52 @@
         <v>3.5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43554</v>
       </c>
+      <c r="B53">
+        <v>6.5</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43555</v>
+      </c>
+      <c r="B54">
+        <v>2.5</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
+      <c r="A55" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43557</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -1218,119 +1246,101 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="D59" s="2" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="D61" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="D63" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="D65" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="D66" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
+      <c r="D67" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="D70" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D78" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D79" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84"/>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completes Week 9 Activity: UserService and UserApplication
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288EA2B5-9DFA-4E76-8A7A-E91B25945982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D9F7A9-7C38-482A-9358-A90105A0B4A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -258,7 +258,12 @@
     <t>Week 9: Activities - finished activities (with question) but not exercise.  See PW answer re: JSON, probably apply in Exercise rather than in activity.</t>
   </si>
   <si>
-    <t>Sun 11 - x Review activity 4 &amp; kelly's work</t>
+    <t>Team Project: looked at what Kelly did (baby web app)
+Week 10: created branch and pull request
+Week 9: worked on activity</t>
+  </si>
+  <si>
+    <t>Finished Week 9 activity</t>
   </si>
 </sst>
 </file>
@@ -629,9 +634,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -1240,13 +1245,26 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43562</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1">
+        <v>43563</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
       <c r="D58" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,80 +1284,101 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="D64" s="2" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="D65" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="D67" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="D69" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="D70" s="2" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="D71" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="D72" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="D74" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="D76" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="D77" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+    <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="2" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempts to correct time log data lost when switching between branch and master.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288EA2B5-9DFA-4E76-8A7A-E91B25945982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3F52A1-C784-4939-92A6-5FD11F5B93EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -258,7 +258,25 @@
     <t>Week 9: Activities - finished activities (with question) but not exercise.  See PW answer re: JSON, probably apply in Exercise rather than in activity.</t>
   </si>
   <si>
-    <t>Sun 11 - x Review activity 4 &amp; kelly's work</t>
+    <t>Team Project: looked at what Kelly did (baby web app)
+Week 10: created branch and pull request
+Week 9: worked on activity</t>
+  </si>
+  <si>
+    <t>Finished Week 9 activity</t>
+  </si>
+  <si>
+    <t>Team project: tried to get log4j out of github; added a service method that provides a party parrot based on name; tried to research some way of handling json info more directly, but did not figure something out so ended up working with a list of all the parrots, as objects, for my method.  
+Issue:Time estimate may be wrong - I lost some time log data while going back and forth between branch and  master of my indie project.</t>
+  </si>
+  <si>
+    <t>early AM - 1 hour, + 8:35 - x</t>
+  </si>
+  <si>
+    <t>created properties file - need to make application upload and use it</t>
+  </si>
+  <si>
+    <t>populated jsp with "top" careers to search</t>
   </si>
 </sst>
 </file>
@@ -629,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,106 +1258,150 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43562</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1">
+        <v>43563</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
       <c r="D58" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43564</v>
+      </c>
+      <c r="B59">
+        <v>4.5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1">
+        <v>43566</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
+      <c r="D62" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
+      <c r="D63" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="D65" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="D67" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
+      <c r="D68" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="D70" s="2" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="D71" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="D73" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="D74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="2" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds passing test demonstrating how to get Web Dev median wage from api call
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3F52A1-C784-4939-92A6-5FD11F5B93EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AAE060-92C4-4684-BC2B-47E66D7EE235}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="5295" yWindow="990" windowWidth="14925" windowHeight="9120" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,13 +270,13 @@
 Issue:Time estimate may be wrong - I lost some time log data while going back and forth between branch and  master of my indie project.</t>
   </si>
   <si>
-    <t>early AM - 1 hour, + 8:35 - x</t>
-  </si>
-  <si>
     <t>created properties file - need to make application upload and use it</t>
   </si>
   <si>
     <t>populated jsp with "top" careers to search</t>
+  </si>
+  <si>
+    <t>early AM - 1 hour, + 8:35 - 11:35 + 8 - x</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,19 +1302,19 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="D62" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="D63" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Enables startup servlet to backfill lucene index and load application properties
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AAE060-92C4-4684-BC2B-47E66D7EE235}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B355A9-4981-498A-87D1-6AB0B6241A02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="990" windowWidth="14925" windowHeight="9120" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -270,13 +270,40 @@
 Issue:Time estimate may be wrong - I lost some time log data while going back and forth between branch and  master of my indie project.</t>
   </si>
   <si>
-    <t>created properties file - need to make application upload and use it</t>
-  </si>
-  <si>
-    <t>populated jsp with "top" careers to search</t>
-  </si>
-  <si>
-    <t>early AM - 1 hour, + 8:35 - 11:35 + 8 - x</t>
+    <t>Indie Project: created properties file; populated JSP with "top" careers to search; played with test to develop logic for getting wage from bls; added method (with hard coded api call for now) to ExperiencesSearch to get a wage for a given career</t>
+  </si>
+  <si>
+    <t>Incorporate properties file into application!</t>
+  </si>
+  <si>
+    <t>Maybe revise how it is constructed?  Dealing with careers on several levels: form display, form value java variable value, code for api call</t>
+  </si>
+  <si>
+    <t>Then make search actually get wages for selected career</t>
+  </si>
+  <si>
+    <t>Next biggie is gathering matching users within 10% of income…</t>
+  </si>
+  <si>
+    <t>Indie Proj - Need to:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Proj - Need to: </t>
+  </si>
+  <si>
+    <t>attemt another method unless Luke gets there first</t>
+  </si>
+  <si>
+    <t>incorporate PW feedback</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>3:30 - x</t>
+  </si>
+  <si>
+    <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.</t>
   </si>
 </sst>
 </file>
@@ -647,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,30 +1318,38 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43566</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43567</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="D62" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="D63" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,79 +1364,136 @@
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="D68" s="2" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
+      <c r="D72" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="D73" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="D75" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="D76" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="D79" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="D80" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="D85" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="2" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
+    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="2" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="2" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="2" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="2" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="2" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lets user select a career and get income info from bls on results page
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B355A9-4981-498A-87D1-6AB0B6241A02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE516119-0798-4ADD-BBC0-32793571920B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -233,12 +233,6 @@
 Indie Project: tried to investigate template security issue… it's the package-lock.json.  Wonder if I could use the template without the javascript and json since it's mostly for layout??  Decided against.  Added header jsp and got rid of random links in jsps.  Developed search jsps and servlets that connect to each other (don't properly handle info yet).  Working on profile jsp and servlet.  working on SurveyDaoTest as part of that.</t>
   </si>
   <si>
-    <t>Note:  I may have needed to do something in web xml to get my application startup servlet to actually load on startup</t>
-  </si>
-  <si>
-    <t>http://tutorials.jenkov.com/java-servlets/web-xml.html</t>
-  </si>
-  <si>
     <t>Indie Project: Cleaning up JSP/Servlet connections, getting rid of hard-coded search stuff, enabling log out.</t>
   </si>
   <si>
@@ -273,15 +267,6 @@
     <t>Indie Project: created properties file; populated JSP with "top" careers to search; played with test to develop logic for getting wage from bls; added method (with hard coded api call for now) to ExperiencesSearch to get a wage for a given career</t>
   </si>
   <si>
-    <t>Incorporate properties file into application!</t>
-  </si>
-  <si>
-    <t>Maybe revise how it is constructed?  Dealing with careers on several levels: form display, form value java variable value, code for api call</t>
-  </si>
-  <si>
-    <t>Then make search actually get wages for selected career</t>
-  </si>
-  <si>
     <t>Next biggie is gathering matching users within 10% of income…</t>
   </si>
   <si>
@@ -297,13 +282,7 @@
     <t>incorporate PW feedback</t>
   </si>
   <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t>3:30 - x</t>
-  </si>
-  <si>
-    <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.</t>
+    <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.  Got the method to get income by career working!  (Needs testing, but initial output looks reasonable)</t>
   </si>
 </sst>
 </file>
@@ -674,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1217,7 @@
         <v>3.5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1249,7 +1228,7 @@
         <v>6.5</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1260,7 +1239,7 @@
         <v>2.5</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1271,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1282,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1293,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1315,7 +1294,7 @@
         <v>4.5</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1326,15 +1305,18 @@
         <v>6</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43567</v>
       </c>
+      <c r="B61">
+        <v>3.5</v>
+      </c>
       <c r="D61" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1343,13 +1325,13 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="D63" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,143 +1339,89 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
+      <c r="D66" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
+      <c r="D67" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="D68" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="D69" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="D70" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="D72" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
+      <c r="D73" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="D75" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="D79" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="D78" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D80" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="D82" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D91" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Successfully adds and tests dao method to get by property range; enables user to retrieve surveys (dump) within 10% range of search income
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE516119-0798-4ADD-BBC0-32793571920B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFCA9B-10F5-4D12-9EC3-D637F78BC363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="2205" yWindow="1470" windowWidth="15195" windowHeight="11730" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Indie Project: created properties file; populated JSP with "top" careers to search; played with test to develop logic for getting wage from bls; added method (with hard coded api call for now) to ExperiencesSearch to get a wage for a given career</t>
   </si>
   <si>
-    <t>Next biggie is gathering matching users within 10% of income…</t>
-  </si>
-  <si>
     <t>Indie Proj - Need to:</t>
   </si>
   <si>
@@ -283,6 +280,22 @@
   </si>
   <si>
     <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.  Got the method to get income by career working!  (Needs testing, but initial output looks reasonable)</t>
+  </si>
+  <si>
+    <t>Testing for methods in ExperiencesSearch</t>
+  </si>
+  <si>
+    <t>Actions for sad path validation in SearchStats and ExperiencesSearcg</t>
+  </si>
+  <si>
+    <t>Add comma to income presentation - try to find int/string manipulation in intro java work!</t>
+  </si>
+  <si>
+    <t>Sat 4:35 - x</t>
+  </si>
+  <si>
+    <t>Deal with this? -- 13-Apr-2019 06:24:39.625 WARNING [localhost-startStop-2] org.apache.catalina.loader.WebappClassLoaderBase.clearReferencesThreads The web application [incomeexperiences] appears to have started a thread named [C3P0PooledConnectionPoolManager[identityToken-&gt;1hgfbpda2682w263f1q0z|7e4e66]-AdminTaskTimer] but has failed to stop it. This is very likely to create a memory leak. Stack trace of thread:
+ java.lang.Object.wait(Native Method)</t>
   </si>
 </sst>
 </file>
@@ -653,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,7 +1329,7 @@
         <v>3.5</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,7 +1338,7 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="D63" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,36 +1349,36 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
+      <c r="D65" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="D66" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="D67" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="D68" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
+      <c r="D69" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="D71" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
@@ -1373,55 +1386,88 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="D73" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="D75" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="D78" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="D80" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="D81" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="82" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="2" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
+    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="2" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="2" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="2" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="2" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="2" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
time log update; pre-deploy commit 4/14
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFCA9B-10F5-4D12-9EC3-D637F78BC363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BEE99B-8182-49FF-A229-D89E926C13A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="1470" windowWidth="15195" windowHeight="11730" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="13425" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Indie Project: created properties file; populated JSP with "top" careers to search; played with test to develop logic for getting wage from bls; added method (with hard coded api call for now) to ExperiencesSearch to get a wage for a given career</t>
   </si>
   <si>
-    <t>Indie Proj - Need to:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Team Proj - Need to: </t>
   </si>
   <si>
@@ -289,20 +286,45 @@
   </si>
   <si>
     <t>Add comma to income presentation - try to find int/string manipulation in intro java work!</t>
-  </si>
-  <si>
-    <t>Sat 4:35 - x</t>
   </si>
   <si>
     <t>Deal with this? -- 13-Apr-2019 06:24:39.625 WARNING [localhost-startStop-2] org.apache.catalina.loader.WebappClassLoaderBase.clearReferencesThreads The web application [incomeexperiences] appears to have started a thread named [C3P0PooledConnectionPoolManager[identityToken-&gt;1hgfbpda2682w263f1q0z|7e4e66]-AdminTaskTimer] but has failed to stop it. This is very likely to create a memory leak. Stack trace of thread:
  java.lang.Object.wait(Native Method)</t>
+  </si>
+  <si>
+    <t>Cleanup:</t>
+  </si>
+  <si>
+    <t>Next:</t>
+  </si>
+  <si>
+    <t>Improve survey getter to retrieve nearest surveys if none in range</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2=Indie Project: Added dao method to get by property range. Application search capability now retrieves surveys within 10% of income input by user (dump only).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3=Parrot project: writing method to get categories, loading properties file and using it to get all the parrots, test shell; challenge - how to set up test "database" with different json file?</t>
+    </r>
+  </si>
+  <si>
+    <t>2:20 = x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,13 +340,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -339,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -350,6 +391,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -666,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="D54" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,10 +1350,10 @@
       <c r="A59" s="1">
         <v>43564</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="3">
         <v>4.5</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1329,46 +1376,44 @@
         <v>3.5</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43568</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="D63" s="2" t="s">
-        <v>82</v>
+      <c r="A63" s="1">
+        <v>43569</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="D64" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="D65" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="D66" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="D67" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
         <v>83</v>
@@ -1376,29 +1421,38 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
+      <c r="D70" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
+      <c r="D71" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
+      <c r="D72" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="D73" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1407,67 +1461,94 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="D78" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
+      <c r="D79" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="D80" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="D81" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="D87" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="2" t="s">
+    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D87" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds and tests(success!) dao method to get surveys by family size and income range
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BEE99B-8182-49FF-A229-D89E926C13A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C638D1-5E6A-4CA9-AC49-B450D7A61ED5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="13425" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="1530" yWindow="435" windowWidth="27240" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -317,7 +317,16 @@
     </r>
   </si>
   <si>
-    <t>2:20 = x</t>
+    <t>Correct survey getter to retrieve only same-family-size surveys</t>
+  </si>
+  <si>
+    <t>Indie project: deployed to AWS with function to target income by career (using bls api), quick test online, then started sketching ideas to build out search</t>
+  </si>
+  <si>
+    <t>Mon AM 45 min</t>
+  </si>
+  <si>
+    <t>Indie project: built and tested doa method that can get surveys by family size AND income range</t>
   </si>
 </sst>
 </file>
@@ -713,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D54" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,25 +1399,36 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43569</v>
       </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1">
+        <v>43570</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="D65" s="2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
+      <c r="D67" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -1422,133 +1442,142 @@
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="D70" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="D72" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="D73" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
+      <c r="D77" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="D79" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="D80" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="D81" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="D84" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="D86" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="D87" s="2" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="D89" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="2" t="s">
+    <row r="90" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="2" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D93" s="2" t="s">
+    <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combines 2 stats searches; starts validation; last commit before refactoring ExperiencesSearch & SearchStats
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C638D1-5E6A-4CA9-AC49-B450D7A61ED5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39EA768-6567-413E-99F5-8B2AC95674C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="435" windowWidth="27240" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -270,9 +270,6 @@
     <t xml:space="preserve">Team Proj - Need to: </t>
   </si>
   <si>
-    <t>attemt another method unless Luke gets there first</t>
-  </si>
-  <si>
     <t>incorporate PW feedback</t>
   </si>
   <si>
@@ -293,12 +290,6 @@
   </si>
   <si>
     <t>Cleanup:</t>
-  </si>
-  <si>
-    <t>Next:</t>
-  </si>
-  <si>
-    <t>Improve survey getter to retrieve nearest surveys if none in range</t>
   </si>
   <si>
     <r>
@@ -317,16 +308,20 @@
     </r>
   </si>
   <si>
-    <t>Correct survey getter to retrieve only same-family-size surveys</t>
-  </si>
-  <si>
     <t>Indie project: deployed to AWS with function to target income by career (using bls api), quick test online, then started sketching ideas to build out search</t>
   </si>
   <si>
-    <t>Mon AM 45 min</t>
-  </si>
-  <si>
     <t>Indie project: built and tested doa method that can get surveys by family size AND income range</t>
+  </si>
+  <si>
+    <t>NEXT: troubleshoot new search, clunky, funky code with not enough exception handling…</t>
+  </si>
+  <si>
+    <t>Tue: ~0.5 + 8:40 - x</t>
+  </si>
+  <si>
+    <t>Week 11: Feedback to presenters
+Indie project: combined 2 search forms and improved search output. Working on validation and refactoring.</t>
   </si>
 </sst>
 </file>
@@ -722,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1380,7 @@
         <v>3.5</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1396,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1407,19 +1402,27 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43570</v>
       </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
       <c r="D64" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43571</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
@@ -1427,7 +1430,7 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="D67" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1436,59 +1439,56 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="D70" s="2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
+      <c r="D72" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="D73" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="D74" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="D76" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="D77" s="2" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
+      <c r="D79" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
@@ -1496,88 +1496,76 @@
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="D81" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="D82" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="D83" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="D86" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="D88" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D89" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D95" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Loads random sample Chart.js chart into statsResult.jsp
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39EA768-6567-413E-99F5-8B2AC95674C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D459ACC9-02CC-48C9-858C-2D8BD494A026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -279,17 +279,8 @@
     <t>Testing for methods in ExperiencesSearch</t>
   </si>
   <si>
-    <t>Actions for sad path validation in SearchStats and ExperiencesSearcg</t>
-  </si>
-  <si>
-    <t>Add comma to income presentation - try to find int/string manipulation in intro java work!</t>
-  </si>
-  <si>
     <t>Deal with this? -- 13-Apr-2019 06:24:39.625 WARNING [localhost-startStop-2] org.apache.catalina.loader.WebappClassLoaderBase.clearReferencesThreads The web application [incomeexperiences] appears to have started a thread named [C3P0PooledConnectionPoolManager[identityToken-&gt;1hgfbpda2682w263f1q0z|7e4e66]-AdminTaskTimer] but has failed to stop it. This is very likely to create a memory leak. Stack trace of thread:
  java.lang.Object.wait(Native Method)</t>
-  </si>
-  <si>
-    <t>Cleanup:</t>
   </si>
   <si>
     <r>
@@ -314,14 +305,20 @@
     <t>Indie project: built and tested doa method that can get surveys by family size AND income range</t>
   </si>
   <si>
-    <t>NEXT: troubleshoot new search, clunky, funky code with not enough exception handling…</t>
-  </si>
-  <si>
-    <t>Tue: ~0.5 + 8:40 - x</t>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>Possible refactoring of statsSearch servlet and testing of removed methods</t>
+  </si>
+  <si>
+    <t>Look into orthodontist problem - income value is "-" with some kind of footnote.  Decide how to handle.</t>
+  </si>
+  <si>
+    <t>Tue: ~0.5 + 8:40 - 3:00</t>
   </si>
   <si>
     <t>Week 11: Feedback to presenters
-Indie project: combined 2 search forms and improved search output. Working on validation and refactoring.</t>
+Indie project: combined 2 search forms and improved search output. Visual testing of validation and flow through program looks ok, except when searching orthodontist.  Still needs unit testing and maybe refactoring.  Also added Chart.js CDN links and random sample chart to my project.</t>
   </si>
 </sst>
 </file>
@@ -719,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
@@ -1391,7 +1388,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1402,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1413,15 +1410,15 @@
         <v>2</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43571</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,7 +1427,7 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="D67" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,40 +1436,30 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
+      <c r="D70" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
       <c r="D72" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="D73" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="D74" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
drafts JSON data for stats charts (needs work); uses better-formatted sample json in js; last commit before deleting commented trials
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D459ACC9-02CC-48C9-858C-2D8BD494A026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4156EC52-2D18-4FE5-9CE6-2F039E268B05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -314,11 +314,8 @@
     <t>Look into orthodontist problem - income value is "-" with some kind of footnote.  Decide how to handle.</t>
   </si>
   <si>
-    <t>Tue: ~0.5 + 8:40 - 3:00</t>
-  </si>
-  <si>
     <t>Week 11: Feedback to presenters
-Indie project: combined 2 search forms and improved search output. Visual testing of validation and flow through program looks ok, except when searching orthodontist.  Still needs unit testing and maybe refactoring.  Also added Chart.js CDN links and random sample chart to my project.</t>
+Indie project: combined 2 search forms and improved search output. Visual testing of validation and flow through program looks ok, except when searching orthodontist.  Still needs unit testing and maybe refactoring.  Also added Chart.js CDN links and random sample chart to my project. Spent quite some time on trying to figure out how to get info into chart; currently stuck</t>
   </si>
 </sst>
 </file>
@@ -1413,12 +1410,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43571</v>
       </c>
+      <c r="B65">
+        <v>9</v>
+      </c>
       <c r="D65" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,9 +1426,6 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="D67" s="2" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>

</xml_diff>

<commit_message>
Displays needs chart without cutting off labels
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4156EC52-2D18-4FE5-9CE6-2F039E268B05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799051BF-29E7-449F-92BD-889B19D0579A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="300" yWindow="660" windowWidth="15870" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -316,6 +316,15 @@
   <si>
     <t>Week 11: Feedback to presenters
 Indie project: combined 2 search forms and improved search output. Visual testing of validation and flow through program looks ok, except when searching orthodontist.  Still needs unit testing and maybe refactoring.  Also added Chart.js CDN links and random sample chart to my project. Spent quite some time on trying to figure out how to get info into chart; currently stuck</t>
+  </si>
+  <si>
+    <t>Indie Project: got real program data into a js chart!</t>
+  </si>
+  <si>
+    <t>Team Project: 6 hrs, testing, refactoring for testable methods, making sure exception handling was done by logging, javadocs, debate/changes to path naming</t>
+  </si>
+  <si>
+    <t>8:30 - x indie: just a tiny bit pm/next am</t>
   </si>
 </sst>
 </file>
@@ -378,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -395,6 +404,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,15 +723,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="115.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="95.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1422,10 +1436,23 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A66" s="1">
+        <v>43572</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43573</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -1433,45 +1460,45 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="D69" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="D70" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="D71" s="2" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="D73" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="D74" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="D79" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1479,77 +1506,92 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="D81" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="D84" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
+      <c r="D85" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="D86" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="D87" s="2" t="s">
+    </row>
+    <row r="88" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="D90" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="D91" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="2" t="s">
+    <row r="92" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="2" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D93" s="2" t="s">
+    <row r="97" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
displays all 3 stats charts from search
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B0B7CE-21AB-4B42-9AF1-0041D7CEA93F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B694B4A-6203-4FCD-976E-BD57B47F972D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -327,10 +327,13 @@
     <t>Team Project: a little more refactoring and re-running javadocs and test results html things</t>
   </si>
   <si>
-    <t xml:space="preserve">Thurs 4:15 - x </t>
-  </si>
-  <si>
-    <t>Update project plan.</t>
+    <t>Thurs 4:15 -6:30</t>
+  </si>
+  <si>
+    <t>Update project plan. Getting all the data needed for charts.</t>
+  </si>
+  <si>
+    <t>8:50 - x</t>
   </si>
 </sst>
 </file>
@@ -731,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:XFD90"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,6 +1518,9 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
+      <c r="D74" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>

</xml_diff>

<commit_message>
adds welcome page to display right after someone signs up
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A697C922-73FF-4AA1-B927-88467F59AC29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1CD6A-CA0E-439A-A367-5F4D137DB80B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -327,7 +327,7 @@
     <t>Team Project: a little more refactoring and re-running javadocs and test results html things</t>
   </si>
   <si>
-    <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality is drafted, not tested.</t>
+    <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality and welcome page are drafted but need to add user role and need to refactor/test.</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,12 +1493,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43580</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
adds role entity, tests role insert, and inserts role when user signs up
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1CD6A-CA0E-439A-A367-5F4D137DB80B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512FD373-9FBB-4A13-B581-705FDDDA42ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="96">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -328,6 +328,24 @@
   </si>
   <si>
     <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality and welcome page are drafted but need to add user role and need to refactor/test.</t>
+  </si>
+  <si>
+    <t>redo role data in clean sql</t>
+  </si>
+  <si>
+    <t>For next deploy I WILL need new database!</t>
+  </si>
+  <si>
+    <t>2019-04-26 15:06:52,445 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
+  </si>
+  <si>
+    <t>^^^ oh hey I just recreated it almost 2 months later!  Maybe it's just occasional</t>
+  </si>
+  <si>
+    <t>Friday 1:40 - 4:40, adding role entity, adding foreign key to db role, debugging breakage (User now needs to be serializable), starting to test, and adding a role upon signup.</t>
+  </si>
+  <si>
+    <t>also rethink roles  - should probably be read, write, and admin.  Then allow users to have multi rows and allow admin to remove roles.</t>
   </si>
 </sst>
 </file>
@@ -364,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +392,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,6 +440,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -726,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,105 +1543,151 @@
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="D73" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="D74" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="D75" s="2" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="D76" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="D78" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="D79" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
+      <c r="D80" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="D83" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="D91" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="D85" s="2" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="D93" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="D86" s="2" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="D94" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D88" s="2" t="s">
+    <row r="95" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="2" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D92" s="2" t="s">
+    <row r="100" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="2" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="2" t="s">
+    <row r="103" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="2" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="2" t="s">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2" t="s">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revised roles structure to read, write, and admin
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512FD373-9FBB-4A13-B581-705FDDDA42ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8488DA7F-4DEA-4D52-AA6A-A35065A5473A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Indie project: built and tested doa method that can get surveys by family size AND income range</t>
   </si>
   <si>
-    <t>TODO:</t>
-  </si>
-  <si>
     <t>Possible refactoring of statsSearch servlet and testing of removed methods</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality and welcome page are drafted but need to add user role and need to refactor/test.</t>
   </si>
   <si>
-    <t>redo role data in clean sql</t>
-  </si>
-  <si>
     <t>For next deploy I WILL need new database!</t>
   </si>
   <si>
@@ -342,10 +336,13 @@
     <t>^^^ oh hey I just recreated it almost 2 months later!  Maybe it's just occasional</t>
   </si>
   <si>
-    <t>Friday 1:40 - 4:40, adding role entity, adding foreign key to db role, debugging breakage (User now needs to be serializable), starting to test, and adding a role upon signup.</t>
-  </si>
-  <si>
-    <t>also rethink roles  - should probably be read, write, and admin.  Then allow users to have multi rows and allow admin to remove roles.</t>
+    <t>adding role entity, adding foreign key to db role, debugging breakage (User now needs to be serializable), starting to test, and adding a role upon signup</t>
+  </si>
+  <si>
+    <t>changing roles and editing db to allow non-unique username in role</t>
+  </si>
+  <si>
+    <t>Next: finish role dao testing.</t>
   </si>
 </sst>
 </file>
@@ -382,7 +379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,12 +398,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -443,9 +434,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -762,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,7 +1470,7 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1493,7 +1481,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1492,7 @@
         <v>2.5</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1515,7 +1503,7 @@
         <v>3.5</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1537,16 +1525,29 @@
         <v>9</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43581</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43584</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
       <c r="D73" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,140 +1555,128 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
+      <c r="D75" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="D76" s="9" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
+      <c r="D77" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="D78" s="10" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="D79" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="D80" s="10" t="s">
-        <v>95</v>
+      <c r="D80" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
+      <c r="D81" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
       <c r="D82" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="D83" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="D85" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="D87" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
+      <c r="D89" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="D91" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="100" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D100" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D101" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="103" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D103" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attempts to let user edit story, work in progress
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8488DA7F-4DEA-4D52-AA6A-A35065A5473A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9C7397-F25B-4861-8484-855B8C856B56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>changing roles and editing db to allow non-unique username in role</t>
-  </si>
-  <si>
-    <t>Next: finish role dao testing.</t>
   </si>
 </sst>
 </file>
@@ -753,7 +750,7 @@
   <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1541,7 @@
         <v>43584</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>93</v>
@@ -1555,9 +1552,6 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="D75" s="2" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>

</xml_diff>

<commit_message>
refactors and tests getSearchResults; currently searches users (to be changed)
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9C7397-F25B-4861-8484-855B8C856B56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC4780-4833-43A9-B00D-3B161B184F78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="660" windowWidth="21540" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t>changing roles and editing db to allow non-unique username in role</t>
+  </si>
+  <si>
+    <t>allowing user to post and revise their financial story; playing with layout; feedback for Andrew (can't find Ciaran's stuff?  - contacted him)</t>
+  </si>
+  <si>
+    <t>gathered some data to add to db before next deploy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Currently stuck on testing that fails for something that DOES work in the application... haven't yet gotten to fixing the presumed bug, which is that I think my application would end up displaying stories that aren't supposed to be visible and/or irrevelavant updated stories from users who at one point had displayed a relevant story. Also attempted to implement some hibernate search filtering, but that was before I realized I probably have a more basic problem.  I think filtering needs to be revised to apply directly to stories, not users. </t>
+  </si>
+  <si>
+    <t>next: check slack for ideas on test problem, consider doing the search revision I think I want (searching stories only) and then re-testing, or at least making sure the application works even if testing doesn't.</t>
   </si>
 </sst>
 </file>
@@ -747,7 +759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
       <selection activeCell="D79" sqref="D79"/>
@@ -1547,63 +1559,87 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43585</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A75" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B76">
+        <v>5.5</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="D77" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
+      <c r="D78" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="D80" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="D81" s="2" t="s">
-        <v>80</v>
+      <c r="D81" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="D89" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,66 +1647,81 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="2" t="s">
+    </row>
+    <row r="93" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="D93" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="D95" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="D96" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D94" s="2" t="s">
+    <row r="97" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="2" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D98" s="2" t="s">
+    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D101" s="2" t="s">
+    <row r="105" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="2" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="2" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="2" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="2" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="2" t="s">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allows user to flag a story in topic search results; works but returns user to failed search screen
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC4780-4833-43A9-B00D-3B161B184F78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DD175-D047-437F-A3A2-3BD403F99550}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -348,10 +348,10 @@
     <t>gathered some data to add to db before next deploy</t>
   </si>
   <si>
-    <t xml:space="preserve">considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Currently stuck on testing that fails for something that DOES work in the application... haven't yet gotten to fixing the presumed bug, which is that I think my application would end up displaying stories that aren't supposed to be visible and/or irrevelavant updated stories from users who at one point had displayed a relevant story. Also attempted to implement some hibernate search filtering, but that was before I realized I probably have a more basic problem.  I think filtering needs to be revised to apply directly to stories, not users. </t>
-  </si>
-  <si>
-    <t>next: check slack for ideas on test problem, consider doing the search revision I think I want (searching stories only) and then re-testing, or at least making sure the application works even if testing doesn't.</t>
+    <t>considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Got stuck on testing - took a while to figure out I needed to set up lucene indexes for the testing db.  Revised search to search for stories, not users, and applied filter so stories have to be visible.</t>
+  </si>
+  <si>
+    <t>Next - get flagging system to work and give admin capacity to work w/ flagged material, especially deleting user.</t>
   </si>
 </sst>
 </file>
@@ -759,9 +759,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
       <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
@@ -1581,12 +1581,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43587</v>
       </c>
       <c r="B76">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>96</v>
@@ -1595,7 +1595,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="D78" s="2" t="s">
         <v>97</v>
@@ -1606,41 +1606,41 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
+      <c r="D80" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="D81" s="9" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
+      <c r="D83" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="D84" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="D89" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
@@ -1648,80 +1648,77 @@
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
+      <c r="D94" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="D95" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="D96" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D98" s="2" t="s">
+    </row>
+    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="2" t="s">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="2" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allows user to flag content without losing info; includes troubleshooting process for trying to redirect back to the same jsp
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DD175-D047-437F-A3A2-3BD403F99550}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA257BA7-0372-4F8A-B1C8-1140681E3649}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -351,7 +351,7 @@
     <t>considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Got stuck on testing - took a while to figure out I needed to set up lucene indexes for the testing db.  Revised search to search for stories, not users, and applied filter so stories have to be visible.</t>
   </si>
   <si>
-    <t>Next - get flagging system to work and give admin capacity to work w/ flagged material, especially deleting user.</t>
+    <t>Got flagging system to work on topics result page.</t>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,13 +1593,18 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="1">
+        <v>43588</v>
+      </c>
+      <c r="B77">
+        <v>3.5</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="D78" s="2" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>

</xml_diff>

<commit_message>
handles the display and flagging of stories the same for both search types
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA257BA7-0372-4F8A-B1C8-1140681E3649}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C367BA-FC8A-4642-8FEF-4539A987B39F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="105" yWindow="660" windowWidth="16470" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>Got flagging system to work on topics result page.</t>
+  </si>
+  <si>
+    <t>TODO - I am using the servlet context in a lot of places where I should be using the session.  Fix that.</t>
+  </si>
+  <si>
+    <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it!</t>
   </si>
 </sst>
 </file>
@@ -759,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,43 +1626,46 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="D83" s="2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="D84" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="D88" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="D92" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1664,66 +1673,81 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="D94" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="D95" s="2" t="s">
+    </row>
+    <row r="96" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="D96" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="D98" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="D99" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D97" s="2" t="s">
+    <row r="100" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D101" s="2" t="s">
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="2" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D104" s="2" t="s">
+    <row r="108" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="2" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds test for finding visible stories flagged for review and sketches admin ideas
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C367BA-FC8A-4642-8FEF-4539A987B39F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7948613-91D8-4462-A08E-AD4D1F858988}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="660" windowWidth="16470" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -351,13 +351,10 @@
     <t>considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Got stuck on testing - took a while to figure out I needed to set up lucene indexes for the testing db.  Revised search to search for stories, not users, and applied filter so stories have to be visible.</t>
   </si>
   <si>
-    <t>Got flagging system to work on topics result page.</t>
-  </si>
-  <si>
-    <t>TODO - I am using the servlet context in a lot of places where I should be using the session.  Fix that.</t>
-  </si>
-  <si>
     <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it!</t>
+  </si>
+  <si>
+    <t>Got flagging system to work on topics result page.  Tested method to get visible unsuitable stories and started sketching out what to do with the admin.</t>
   </si>
 </sst>
 </file>
@@ -765,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,15 +1595,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43588</v>
       </c>
       <c r="B77">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,14 +1624,11 @@
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="D82" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="D83" s="2" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
@@ -1644,29 +1638,29 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="D87" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
       <c r="D88" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="D91" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
@@ -1674,80 +1668,77 @@
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="D96" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
+      <c r="D97" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="D98" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-      <c r="D99" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D101" s="2" t="s">
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="2" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="2" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="2" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
conveys needed info from admin servlet to jsp
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7948613-91D8-4462-A08E-AD4D1F858988}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F968B-5C40-4FFF-B73A-C4DAE9C5722C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="660" windowWidth="16470" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Got flagging system to work on topics result page.  Tested method to get visible unsuitable stories and started sketching out what to do with the admin.</t>
+  </si>
+  <si>
+    <t>Adds dao method to tally entities by multiple criteria.  Tests the method and drafts its use in gathering info for the admin page. Attempts sending info to jsp in a set of maps; not working, probably need to add set to user.  Could just add getter for number of bad histories and put that in the user entity.  Then send users to jsp instead of stories? Send both?</t>
   </si>
 </sst>
 </file>
@@ -762,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,139 +1609,156 @@
         <v>98</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B78">
+        <v>2.5</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="D80" s="9" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="D82" s="2" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
+      <c r="D83" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
+      <c r="D85" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="D86" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="D87" s="2" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="D89" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="D90" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="2" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="D91" s="2" t="s">
+    <row r="94" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="D94" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="D95" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="D97" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="D98" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="D100" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="D101" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D100" s="2" t="s">
+    <row r="102" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D104" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D107" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="2" t="s">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enables admin to remove a user.  messy admin interface.
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F968B-5C40-4FFF-B73A-C4DAE9C5722C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDCAA0B-EF2D-42C9-96D8-2BEBC010FEE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="660" windowWidth="16470" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="105" yWindow="660" windowWidth="28620" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,13 +351,13 @@
     <t>considered how admin page should work in light of general scaling back.  Found an api of interest for working with "bad" words but probably won't implement.  Uncovered what I think is an error in my search-by-topic page, which led to some refactoring and testing.  Got stuck on testing - took a while to figure out I needed to set up lucene indexes for the testing db.  Revised search to search for stories, not users, and applied filter so stories have to be visible.</t>
   </si>
   <si>
-    <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it!</t>
-  </si>
-  <si>
     <t>Got flagging system to work on topics result page.  Tested method to get visible unsuitable stories and started sketching out what to do with the admin.</t>
   </si>
   <si>
     <t>Adds dao method to tally entities by multiple criteria.  Tests the method and drafts its use in gathering info for the admin page. Attempts sending info to jsp in a set of maps; not working, probably need to add set to user.  Could just add getter for number of bad histories and put that in the user entity.  Then send users to jsp instead of stories? Send both?</t>
+  </si>
+  <si>
+    <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it! Hahahahahaha</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1606,7 @@
         <v>5.5</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1614,10 +1614,10 @@
         <v>43589</v>
       </c>
       <c r="B78">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds some layout features
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDCAA0B-EF2D-42C9-96D8-2BEBC010FEE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180841A-6741-439B-A0C0-351F9E08482F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="660" windowWidth="28620" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -354,10 +354,10 @@
     <t>Got flagging system to work on topics result page.  Tested method to get visible unsuitable stories and started sketching out what to do with the admin.</t>
   </si>
   <si>
-    <t>Adds dao method to tally entities by multiple criteria.  Tests the method and drafts its use in gathering info for the admin page. Attempts sending info to jsp in a set of maps; not working, probably need to add set to user.  Could just add getter for number of bad histories and put that in the user entity.  Then send users to jsp instead of stories? Send both?</t>
-  </si>
-  <si>
     <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it! Hahahahahaha</t>
+  </si>
+  <si>
+    <t>Added a dao method to tally entities by multiple criteria (and now realize I'm not going to use it!). Created separate getter method in user to tally hidden "unsuitable" stories. Implemented admin's ability to remove a user and set up display for admin to be able to take other actions when shown flagged content.  Did a little work with front end.</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,10 +1614,10 @@
         <v>43589</v>
       </c>
       <c r="B78">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds and tests method to check whether a user has write privileges
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180841A-6741-439B-A0C0-351F9E08482F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B932FC12-C4EB-4D49-B7EC-9F225694F870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="660" windowWidth="28620" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t>Added a dao method to tally entities by multiple criteria (and now realize I'm not going to use it!). Created separate getter method in user to tally hidden "unsuitable" stories. Implemented admin's ability to remove a user and set up display for admin to be able to take other actions when shown flagged content.  Did a little work with front end.</t>
+  </si>
+  <si>
+    <t>Sun am - 3 - allows admin to unflag a story or block a user and hide their stories.</t>
+  </si>
+  <si>
+    <t>Need blocked user to actually not be able to write</t>
+  </si>
+  <si>
+    <t>Next biggest issue is validation, I think, and of course interface.</t>
   </si>
 </sst>
 </file>
@@ -768,7 +777,7 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,10 +1630,15 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="1">
+        <v>43590</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
+      <c r="D80" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
@@ -1649,9 +1663,15 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>

</xml_diff>

<commit_message>
enables admin to block a user by fixing the method to remove write privilege; actually does stop user from writing a story now
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B932FC12-C4EB-4D49-B7EC-9F225694F870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C9D74E-FD1C-48E2-BD75-B3478097F237}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="660" windowWidth="28620" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -363,10 +363,13 @@
     <t>Sun am - 3 - allows admin to unflag a story or block a user and hide their stories.</t>
   </si>
   <si>
-    <t>Need blocked user to actually not be able to write</t>
-  </si>
-  <si>
     <t>Next biggest issue is validation, I think, and of course interface.</t>
+  </si>
+  <si>
+    <t>For db - add read write ability to admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added capability for an admin to unflag a story or block a user and hide their story.  </t>
   </si>
 </sst>
 </file>
@@ -774,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,39 +1636,39 @@
       <c r="A79" s="1">
         <v>43590</v>
       </c>
+      <c r="B79">
+        <v>4.5</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="D80" s="2" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="D83" s="9" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="D85" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="D86" s="2" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
@@ -1679,106 +1682,121 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="D89" s="2" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="D90" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="D92" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="D93" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="2" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="D94" s="2" t="s">
+    <row r="97" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="D97" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
-      <c r="D98" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="D100" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="D101" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="D103" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="D104" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D103" s="2" t="s">
+    <row r="105" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D107" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D110" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D111" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="2" t="s">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactors signup servlet - adds logic class; also a little cleanup
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C9D74E-FD1C-48E2-BD75-B3478097F237}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559E9345-9E99-46E8-A57A-700AA97738C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="660" windowWidth="28620" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="2940" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
     <t>For db - add read write ability to admin</t>
   </si>
   <si>
-    <t xml:space="preserve">Added capability for an admin to unflag a story or block a user and hide their story.  </t>
+    <t>Added capability for an admin to unflag a story or block a user and hide their story.  Refactors signup servlet, adds logic class, sets up jsp to present previously entered username if signup fails - other fields need to be set up too.</t>
   </si>
 </sst>
 </file>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,12 +1632,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43590</v>
       </c>
       <c r="B79">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
adds intermediate work before bigger refactor of SearchStats and ExperiencesSearch
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559E9345-9E99-46E8-A57A-700AA97738C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68DF18E-27F0-4F11-A928-FF196FC522DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="5955" yWindow="15" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -360,9 +365,6 @@
     <t>Added a dao method to tally entities by multiple criteria (and now realize I'm not going to use it!). Created separate getter method in user to tally hidden "unsuitable" stories. Implemented admin's ability to remove a user and set up display for admin to be able to take other actions when shown flagged content.  Did a little work with front end.</t>
   </si>
   <si>
-    <t>Sun am - 3 - allows admin to unflag a story or block a user and hide their stories.</t>
-  </si>
-  <si>
     <t>Next biggest issue is validation, I think, and of course interface.</t>
   </si>
   <si>
@@ -370,6 +372,33 @@
   </si>
   <si>
     <t>Added capability for an admin to unflag a story or block a user and hide their story.  Refactors signup servlet, adds logic class, sets up jsp to present previously entered username if signup fails - other fields need to be set up too.</t>
+  </si>
+  <si>
+    <t>Completed backend validation of signup, then applied html restrictions.</t>
+  </si>
+  <si>
+    <t>goals before class</t>
+  </si>
+  <si>
+    <t>better search validation similar to sign-up: message at top, required household size, deal with orthodontist npe</t>
+  </si>
+  <si>
+    <t>get db in good enough shape to deploy (not necessarily additional data)</t>
+  </si>
+  <si>
+    <t>deploy</t>
+  </si>
+  <si>
+    <t>sketch goals for review - Kelly shouldn't have to comb through all this!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if time, refactor searching servlets and logic </t>
+  </si>
+  <si>
+    <t>defer testing til later.</t>
+  </si>
+  <si>
+    <t>do I need to redo the robo pojo thing for to accommodate footnotes???  (see log)</t>
   </si>
 </sst>
 </file>
@@ -777,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,40 +1669,54 @@
         <v>7.5</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>43591</v>
+      </c>
+      <c r="B80">
+        <v>1.5</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="D82" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="D85" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="D87" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,121 +1725,163 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="D90" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
+      <c r="D91" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="D93" s="2" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="D96" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="D97" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
+      <c r="D98" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
+      <c r="D99" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="D101" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
+      <c r="D102" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
       <c r="D103" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="D106" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="D110" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="D112" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="D104" s="2" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="D113" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D106" s="2" t="s">
+    <row r="114" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="2" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D110" s="2" t="s">
+    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="2" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D113" s="2" t="s">
+    <row r="122" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="2" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="2" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="2" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="2" t="s">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="2" t="s">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactors SearchStats and ExpriencesSearch moving more logic out of the servlet
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68DF18E-27F0-4F11-A928-FF196FC522DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD346F60-BCB0-4DF9-8893-0788B6EDAE8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5955" yWindow="15" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -374,9 +374,6 @@
     <t>Added capability for an admin to unflag a story or block a user and hide their story.  Refactors signup servlet, adds logic class, sets up jsp to present previously entered username if signup fails - other fields need to be set up too.</t>
   </si>
   <si>
-    <t>Completed backend validation of signup, then applied html restrictions.</t>
-  </si>
-  <si>
     <t>goals before class</t>
   </si>
   <si>
@@ -399,6 +396,12 @@
   </si>
   <si>
     <t>do I need to redo the robo pojo thing for to accommodate footnotes???  (see log)</t>
+  </si>
+  <si>
+    <t>TODO NOW INCOME NEEDS TO BE A LONG!</t>
+  </si>
+  <si>
+    <t>Completed backend validation of signup, then applied html restrictions. Big refactor of Stats Search servlet &amp; logic class.  Also started looking into dealing with orthodontist - didn't get very far.</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,6 +493,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,15 +1678,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43591</v>
       </c>
       <c r="B80">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,122 +1694,125 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="D82" s="9" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="D83" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="D84" s="2" t="s">
-        <v>104</v>
+      <c r="D84" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="D86" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="D87" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="D89" s="2" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="D90" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="D91" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
+      <c r="D92" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="2" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
+      <c r="D94" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="D96" s="2" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
+      <c r="D97" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
-      <c r="D98" s="2" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="D99" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
+      <c r="D100" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
-      <c r="D101" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="D102" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="D103" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="2" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="D106" s="2" t="s">
+    <row r="107" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="D107" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
@@ -1811,77 +1820,80 @@
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="D110" s="2" t="s">
+    </row>
+    <row r="111" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="D111" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="D112" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="D113" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="D114" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D115" s="2" t="s">
+    <row r="115" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="2" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D119" s="2" t="s">
+    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="2" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D122" s="2" t="s">
+    <row r="123" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="2" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="2" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D128" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="2" t="s">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates problem statement for current scope; adds info to index
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD346F60-BCB0-4DF9-8893-0788B6EDAE8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEDC7C2-6B7E-4210-A3EA-667FB19CAE8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="15" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="7395" yWindow="8625" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -332,9 +332,6 @@
     <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality and welcome page are drafted but need to add user role and need to refactor/test.</t>
   </si>
   <si>
-    <t>For next deploy I WILL need new database!</t>
-  </si>
-  <si>
     <t>2019-04-26 15:06:52,445 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
   </si>
   <si>
@@ -359,49 +356,28 @@
     <t>Got flagging system to work on topics result page.  Tested method to get visible unsuitable stories and started sketching out what to do with the admin.</t>
   </si>
   <si>
-    <t>NB - the topic search results really aren't very useful without a profile link - I should do it if I can manage it! Hahahahahaha</t>
-  </si>
-  <si>
     <t>Added a dao method to tally entities by multiple criteria (and now realize I'm not going to use it!). Created separate getter method in user to tally hidden "unsuitable" stories. Implemented admin's ability to remove a user and set up display for admin to be able to take other actions when shown flagged content.  Did a little work with front end.</t>
   </si>
   <si>
     <t>Next biggest issue is validation, I think, and of course interface.</t>
   </si>
   <si>
-    <t>For db - add read write ability to admin</t>
-  </si>
-  <si>
     <t>Added capability for an admin to unflag a story or block a user and hide their story.  Refactors signup servlet, adds logic class, sets up jsp to present previously entered username if signup fails - other fields need to be set up too.</t>
   </si>
   <si>
-    <t>goals before class</t>
-  </si>
-  <si>
-    <t>better search validation similar to sign-up: message at top, required household size, deal with orthodontist npe</t>
-  </si>
-  <si>
-    <t>get db in good enough shape to deploy (not necessarily additional data)</t>
-  </si>
-  <si>
-    <t>deploy</t>
-  </si>
-  <si>
-    <t>sketch goals for review - Kelly shouldn't have to comb through all this!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if time, refactor searching servlets and logic </t>
-  </si>
-  <si>
-    <t>defer testing til later.</t>
-  </si>
-  <si>
-    <t>do I need to redo the robo pojo thing for to accommodate footnotes???  (see log)</t>
-  </si>
-  <si>
-    <t>TODO NOW INCOME NEEDS TO BE A LONG!</t>
-  </si>
-  <si>
     <t>Completed backend validation of signup, then applied html restrictions. Big refactor of Stats Search servlet &amp; logic class.  Also started looking into dealing with orthodontist - didn't get very far.</t>
+  </si>
+  <si>
+    <t>check db in deploy:</t>
+  </si>
+  <si>
+    <t>TODO NOW INCOME NEEDS TO BE A LONG! - although I don't seem to have problems yet?</t>
+  </si>
+  <si>
+    <t>Reviewed Kelly's project.</t>
+  </si>
+  <si>
+    <t>11:30 - x indie project</t>
   </si>
 </sst>
 </file>
@@ -470,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,9 +466,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -812,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1571,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1609,7 +1582,7 @@
         <v>1.5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1620,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1642,7 +1615,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1653,7 +1626,7 @@
         <v>5.5</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1664,7 +1637,7 @@
         <v>6.5</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1675,7 +1648,7 @@
         <v>7.5</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1686,49 +1659,47 @@
         <v>5</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+      <c r="A81" s="1">
+        <v>43592</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="D83" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="D84" s="10" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="D85" s="2" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="D86" s="2" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="D87" s="2" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="D88" s="2" t="s">
-        <v>109</v>
+      <c r="A88" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,164 +1707,126 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="D90" s="2" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="D91" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="2" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
+      <c r="D93" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="D94" s="2" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
+      <c r="D95" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="D97" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="D99" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="D100" s="2" t="s">
-        <v>100</v>
+    </row>
+    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="D102" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
-      <c r="D103" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
       <c r="D104" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="D105" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="D107" s="2" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
+      <c r="D109" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D111" s="2" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="D113" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
+      <c r="D112" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D114" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D116" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allows search jsp to retain inputs when invalid; adds a few javadoc comments
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEDC7C2-6B7E-4210-A3EA-667FB19CAE8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2329343-AFF3-488B-B520-EDC0FF58DD6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="8625" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="7395" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -374,10 +374,16 @@
     <t>TODO NOW INCOME NEEDS TO BE A LONG! - although I don't seem to have problems yet?</t>
   </si>
   <si>
-    <t>Reviewed Kelly's project.</t>
-  </si>
-  <si>
-    <t>11:30 - x indie project</t>
+    <t>Reviewed Kelly's project. Mostly finished front end of Indie project.</t>
+  </si>
+  <si>
+    <t>Looked into why new stories weren't searchable on aws.</t>
+  </si>
+  <si>
+    <t>3:45 - x</t>
+  </si>
+  <si>
+    <t>Revised search jsp to hold inputs when search validation failed.</t>
   </si>
 </sst>
 </file>
@@ -787,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
       <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
@@ -1667,19 +1673,29 @@
         <v>43592</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+      <c r="A82" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1">
+        <v>43594</v>
+      </c>
       <c r="D83" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,6 +1703,9 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
+      <c r="D85" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>

</xml_diff>

<commit_message>
refactored some ExperiencesSearch methods to ChartData.js; search still works
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2329343-AFF3-488B-B520-EDC0FF58DD6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A490E5C-F898-44CF-A054-68803E12D548}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7395" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.  Got the method to get income by career working!  (Needs testing, but initial output looks reasonable)</t>
-  </si>
-  <si>
-    <t>Testing for methods in ExperiencesSearch</t>
   </si>
   <si>
     <t>Deal with this? -- 13-Apr-2019 06:24:39.625 WARNING [localhost-startStop-2] org.apache.catalina.loader.WebappClassLoaderBase.clearReferencesThreads The web application [incomeexperiences] appears to have started a thread named [C3P0PooledConnectionPoolManager[identityToken-&gt;1hgfbpda2682w263f1q0z|7e4e66]-AdminTaskTimer] but has failed to stop it. This is very likely to create a memory leak. Stack trace of thread:
@@ -304,12 +301,6 @@
     <t>Indie project: built and tested doa method that can get surveys by family size AND income range</t>
   </si>
   <si>
-    <t>Possible refactoring of statsSearch servlet and testing of removed methods</t>
-  </si>
-  <si>
-    <t>Look into orthodontist problem - income value is "-" with some kind of footnote.  Decide how to handle.</t>
-  </si>
-  <si>
     <t>Week 11: Feedback to presenters
 Indie project: combined 2 search forms and improved search output. Visual testing of validation and flow through program looks ok, except when searching orthodontist.  Still needs unit testing and maybe refactoring.  Also added Chart.js CDN links and random sample chart to my project. Spent quite some time on trying to figure out how to get info into chart; currently stuck</t>
   </si>
@@ -359,9 +350,6 @@
     <t>Added a dao method to tally entities by multiple criteria (and now realize I'm not going to use it!). Created separate getter method in user to tally hidden "unsuitable" stories. Implemented admin's ability to remove a user and set up display for admin to be able to take other actions when shown flagged content.  Did a little work with front end.</t>
   </si>
   <si>
-    <t>Next biggest issue is validation, I think, and of course interface.</t>
-  </si>
-  <si>
     <t>Added capability for an admin to unflag a story or block a user and hide their story.  Refactors signup servlet, adds logic class, sets up jsp to present previously entered username if signup fails - other fields need to be set up too.</t>
   </si>
   <si>
@@ -371,19 +359,16 @@
     <t>check db in deploy:</t>
   </si>
   <si>
-    <t>TODO NOW INCOME NEEDS TO BE A LONG! - although I don't seem to have problems yet?</t>
-  </si>
-  <si>
     <t>Reviewed Kelly's project. Mostly finished front end of Indie project.</t>
   </si>
   <si>
     <t>Looked into why new stories weren't searchable on aws.</t>
   </si>
   <si>
-    <t>3:45 - x</t>
-  </si>
-  <si>
     <t>Revised search jsp to hold inputs when search validation failed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:30 - x </t>
   </si>
 </sst>
 </file>
@@ -420,7 +405,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,12 +415,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -794,7 +773,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1446,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1478,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1500,7 +1479,7 @@
         <v>9</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1522,7 +1501,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,7 +1512,7 @@
         <v>2.5</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1544,7 +1523,7 @@
         <v>3.5</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1566,7 +1545,7 @@
         <v>9</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1577,7 +1556,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,7 +1567,7 @@
         <v>1.5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1599,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1610,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1621,7 +1600,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1632,7 +1611,7 @@
         <v>5.5</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1643,7 +1622,7 @@
         <v>6.5</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1654,7 +1633,7 @@
         <v>7.5</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1665,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,7 +1655,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,15 +1666,18 @@
         <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43594</v>
       </c>
+      <c r="B83">
+        <v>2.5</v>
+      </c>
       <c r="D83" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,7 +1686,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="D85" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,54 +1697,48 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>102</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D88" s="9"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
+      <c r="D89" s="9"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
+      <c r="D90" s="9"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="D91" s="9"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
+      <c r="D92" s="9"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D93" s="9"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="D94" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="D94" s="9"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="D95" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="D95" s="9"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
+      <c r="D96" s="9"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
     <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,12 +1796,12 @@
     </row>
     <row r="114" spans="4:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D114" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adds ddl for test and production databases
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A490E5C-F898-44CF-A054-68803E12D548}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C4040F-2043-4002-86F8-FE5DA7EC4F77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -356,19 +356,43 @@
     <t>Completed backend validation of signup, then applied html restrictions. Big refactor of Stats Search servlet &amp; logic class.  Also started looking into dealing with orthodontist - didn't get very far.</t>
   </si>
   <si>
-    <t>check db in deploy:</t>
-  </si>
-  <si>
     <t>Reviewed Kelly's project. Mostly finished front end of Indie project.</t>
   </si>
   <si>
     <t>Looked into why new stories weren't searchable on aws.</t>
   </si>
   <si>
-    <t>Revised search jsp to hold inputs when search validation failed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:30 - x </t>
+    <t>Revised search jsp to hold inputs when search validation failed. Refactored code to reduce class and method size. Started testing methods to get chart data.</t>
+  </si>
+  <si>
+    <t>Added data to database locally.</t>
+  </si>
+  <si>
+    <t>Fri plan</t>
+  </si>
+  <si>
+    <t>Make new users to demo a cluster of data; add via program.</t>
+  </si>
+  <si>
+    <t>Make new users have interesting stories.</t>
+  </si>
+  <si>
+    <t>Choose searches  to demo.</t>
+  </si>
+  <si>
+    <t>1. retrieve cluster by career and family size</t>
+  </si>
+  <si>
+    <t>3. attempt retrieval with no results</t>
+  </si>
+  <si>
+    <t>a. orthodontist to demo failed api search</t>
+  </si>
+  <si>
+    <t>b. another one with no data cluster.</t>
+  </si>
+  <si>
+    <t>2. retrieve whatever possible that requires 30% search</t>
   </si>
 </sst>
 </file>
@@ -773,7 +797,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1679,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1666,40 +1690,51 @@
         <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43594</v>
       </c>
       <c r="B83">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="D83" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="D85" s="2" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" s="9"/>
+      <c r="A88" s="1"/>
+      <c r="D88" s="9" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
@@ -1707,27 +1742,39 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="D90" s="9"/>
+      <c r="D90" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="9"/>
+      <c r="D91" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="9"/>
+      <c r="D92" s="9" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="9"/>
+      <c r="D93" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="D94" s="9"/>
+      <c r="D94" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="D95" s="9"/>
+      <c r="D95" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>

</xml_diff>

<commit_message>
fixes ExperienceSearch to allow search by income again
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C4040F-2043-4002-86F8-FE5DA7EC4F77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BEB79B-6549-4BBE-A81B-95DC05D6B293}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Choose searches  to demo.</t>
   </si>
   <si>
-    <t>1. retrieve cluster by career and family size</t>
-  </si>
-  <si>
     <t>3. attempt retrieval with no results</t>
   </si>
   <si>
@@ -392,7 +389,13 @@
     <t>b. another one with no data cluster.</t>
   </si>
   <si>
-    <t>2. retrieve whatever possible that requires 30% search</t>
+    <t>2. retrieve whatever possible that requires 30% search: software developer, family of 6</t>
+  </si>
+  <si>
+    <t>1. retrieve cluster by career and family size:  $50k, familly of 2</t>
+  </si>
+  <si>
+    <t>FIX income search!!</t>
   </si>
 </sst>
 </file>
@@ -794,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,148 +1730,157 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="D87" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="D88" s="9" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="D89" s="9"/>
+      <c r="D89" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="D90" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="D91" s="9"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="D92" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="D93" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="D94" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="D95" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="D96" s="9"/>
+      <c r="D96" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="D98" s="2" t="s">
+      <c r="D97" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="D98" s="9"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="D102" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="D104" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="D105" s="2" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
+      <c r="D106" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="D107" s="2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="D109" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="D111" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D111" s="2" t="s">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="2" t="s">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D114" s="2" t="s">
+    <row r="116" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="2" t="s">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="117" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
+    <row r="119" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes problem working with stories with quotes by using ids, not content, to work with them
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9B8E76-CD8F-4BAE-AD01-E8A14860680B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84594F99-2F2E-4523-941F-A81CA8377C3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -428,7 +428,10 @@
     <t>2. Attempt to use admin - shouldn't work.</t>
   </si>
   <si>
-    <t>sat &lt;3 early am</t>
+    <t>worked on presentation (getting to know obs software, making powerpoint, planning flow)</t>
+  </si>
+  <si>
+    <t>Adding data to deployed application, troubleshooting a crash</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
       <selection activeCell="D87" sqref="D87"/>
@@ -1763,12 +1766,25 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="A85" s="1">
+        <v>43596</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="A86" s="1">
+        <v>43597</v>
+      </c>
+      <c r="B86">
+        <v>1.5</v>
+      </c>
       <c r="D86" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1776,162 +1792,156 @@
     </row>
     <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="D88" s="10" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="D89" s="2" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="D90" s="2" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="2" t="s">
-        <v>110</v>
+      <c r="D91" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="D92" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="D93" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="D94" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="D95" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="D96" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="D97" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="D98" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="D99" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="D98" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="D99" s="9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="D100" s="9" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="D101" s="9" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="D102" s="9" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="D103" s="9" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="D104" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="D105" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="D106" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="D107" s="9" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="D108" s="9" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-      <c r="D109" s="9"/>
+      <c r="D109" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="D110" s="9"/>
-    </row>
-    <row r="111" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="D111" s="2" t="s">
+      <c r="D110" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="D111" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="D112" s="9"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="D113" s="9"/>
+    </row>
+    <row r="114" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="D115" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="D117" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="D118" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,57 +1950,72 @@
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="D120" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
-      <c r="D122" s="2" t="s">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="D123" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="D125" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D124" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D127" s="2" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D128" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D130" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="2" t="s">
+    <row r="133" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds javadocs, adds slideshow (in progress), updates readme
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84594F99-2F2E-4523-941F-A81CA8377C3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90E1226-17AF-4EA1-871D-9103401808BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -365,33 +365,9 @@
     <t>Revised search jsp to hold inputs when search validation failed. Refactored code to reduce class and method size. Started testing methods to get chart data.</t>
   </si>
   <si>
-    <t>3. attempt retrieval with no results</t>
-  </si>
-  <si>
-    <t>a. orthodontist to demo failed api search</t>
-  </si>
-  <si>
-    <t>2. retrieve whatever possible that requires 30% search: software developer, family of 6</t>
-  </si>
-  <si>
-    <t>1. retrieve cluster by career and family size:  $50k, familly of 2</t>
-  </si>
-  <si>
-    <t>4. search for child care</t>
-  </si>
-  <si>
-    <t>b. another one with no data cluster. - 300000, family of 3</t>
-  </si>
-  <si>
     <t>Added data to database, found software for screencast, fixed a search validation problem.</t>
   </si>
   <si>
-    <t>File by file - javadocs, unused stuff, todos</t>
-  </si>
-  <si>
-    <t>Powerpoint shell - figure how much is in video, what is in ppt: also where will project link javadocs?</t>
-  </si>
-  <si>
     <t>Weekend</t>
   </si>
   <si>
@@ -413,25 +389,13 @@
     <t>Make javadocs - need to be on GitHub, maybe add link to ReadMe</t>
   </si>
   <si>
-    <t>5.Demo flagging</t>
-  </si>
-  <si>
-    <t>6.Demo admin actions</t>
-  </si>
-  <si>
-    <t>Demo</t>
-  </si>
-  <si>
-    <t>1. Sign in as new user and log in.  Make 1-2 sign up mistakes at first to show how validation generally looks.</t>
-  </si>
-  <si>
-    <t>2. Attempt to use admin - shouldn't work.</t>
-  </si>
-  <si>
     <t>worked on presentation (getting to know obs software, making powerpoint, planning flow)</t>
   </si>
   <si>
-    <t>Adding data to deployed application, troubleshooting a crash</t>
+    <t>Adding data to deployed application, troubleshooting a crash, and another one. Making the video demo.</t>
+  </si>
+  <si>
+    <t>8:10 - x</t>
   </si>
 </sst>
 </file>
@@ -502,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -522,9 +486,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,7 +1723,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,7 +1734,7 @@
         <v>5</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,10 +1742,10 @@
         <v>43597</v>
       </c>
       <c r="B86">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1795,227 +1756,150 @@
     </row>
     <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
+      <c r="D89" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
     <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="10" t="s">
-        <v>109</v>
+      <c r="D91" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="D92" s="2" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
-      <c r="D93" s="2" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="D94" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="D95" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="D96" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="D97" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="D98" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="D99" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="D101" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="D102" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="D103" s="9" t="s">
-        <v>120</v>
+    <row r="101" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
-      <c r="D104" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="D105" s="9" t="s">
-        <v>102</v>
+      <c r="D105" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
-      <c r="D106" s="9" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="D107" s="9" t="s">
-        <v>101</v>
+      <c r="D107" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
-      <c r="D108" s="9" t="s">
-        <v>105</v>
+      <c r="D108" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-      <c r="D109" s="9" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="D110" s="9" t="s">
-        <v>116</v>
+      <c r="D110" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
-      <c r="D111" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="D112" s="9"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="D113" s="9"/>
-    </row>
-    <row r="114" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="4:4" ht="45" x14ac:dyDescent="0.25">
       <c r="D114" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="D120" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-      <c r="D121" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-      <c r="D125" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D127" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="130" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D130" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="133" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="2" t="s">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="2" t="s">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completes PowerPoint with current testing numbers
</commit_message>
<xml_diff>
--- a/EnterpriseJavaTimeLog.xlsx
+++ b/EnterpriseJavaTimeLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idile\IdeaProjects\incomeexperiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90E1226-17AF-4EA1-871D-9103401808BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159FC5EE-B2A6-42E3-A1F1-B92BDBB4DD0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
+    <workbookView xWindow="7395" yWindow="660" windowWidth="16380" windowHeight="14940" xr2:uid="{3162A6E2-721B-4438-91B4-1225751973F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Time Log Enterprise Java</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Indie Project: setting up test database, properties, copying Database class, creating sql for cleaning database before testing, starting UserDaoTest, setting up log4j properties, changing mysql username and pw, trying to delete sensitive files from GitHub, troubleshooting why my cleandb.sql isn't actually running...</t>
-  </si>
-  <si>
-    <t>NB: new password so files/setup need to change in prior repos</t>
   </si>
   <si>
     <t>Week 4ish: Getting passwords out of repo for Week 1 exercise
@@ -128,9 +125,6 @@
 Week 5: started videos</t>
   </si>
   <si>
-    <t>Issues/Loose Ends:</t>
-  </si>
-  <si>
     <t>Week 4/Project: Completed Exercise 4 with javadocs and test results. Looked into question of what exactly session.save(object) returns.
 Week 5: Finished videos, reading (but would like to re-read the equals thing</t>
   </si>
@@ -141,19 +135,7 @@
     <t>Resolved Log4J issue rolling files.  Feedback on presentation (yesterday).  Finished annotations for Story class and associating User and Story.  Generated basic functions for Story.</t>
   </si>
   <si>
-    <t>Removed from UserDao comments -- save for a later time, differetn place</t>
-  </si>
-  <si>
     <t>Setting up and testing remaining methods for User, StoryDao testing, looking into date conversions (turned out to be unnecessary).</t>
-  </si>
-  <si>
-    <t>2019-03-01 06:11:44,732 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
-  </si>
-  <si>
-    <t>Useful mysql tutorial: used for changing foreign key constraint:</t>
-  </si>
-  <si>
-    <t>http://www.mysqltutorial.org/mysql-foreign-key/</t>
   </si>
   <si>
     <t>Indie Project: figuring out getByProperty issue in StoryDaoTest; reviewing generic dao examples; worked on testing effects of insert and delete on associated entities; finished tests for User, UserDao, and StoryDao
@@ -172,12 +154,6 @@
   <si>
     <t>Indie Project: organized priorities, figured out how to generate UML diagrams from IntelliJ, tried and failed to recreate Log4J problem, set up Servlet shells and super basic entity classes
 Week 7: Intro video</t>
-  </si>
-  <si>
-    <t>TODO (nice to do)  -  refactor tests to use .equals in UserDaoTest and StoryDaoTest</t>
-  </si>
-  <si>
-    <t>^^^ Recently unable to re-create</t>
   </si>
   <si>
     <t>Indie Project: consider how logic class will work - is it really a special dao?; revised database design and associated classes; implemented GenericDao, started a profile JSP</t>
@@ -219,9 +195,6 @@
 Fixed config so it doesn't kill my program.  Attempted a hibernate search - not getting expected result yet.</t>
   </si>
   <si>
-    <t>TODO-- Week 7 see PW snippet for better servlet mapping</t>
-  </si>
-  <si>
     <t>Project/Presentation: Got code working to backfill the indexes for Hibernate Search; completed several kinds of searchs; completed presentation materials</t>
   </si>
   <si>
@@ -229,9 +202,6 @@
   </si>
   <si>
     <t>Week 8 Activities (including time spent sorting out how to handle file permissions in jdk lib)</t>
-  </si>
-  <si>
-    <t>TODO-- PW feedback authentication You may find that to get very fine-grained control over specific data when using a servlet that serve a couple different user types (view my profile versus view somebody else's profile), you may want to check the role within the servlet. The other option would be to set up two servlets ViewMyProfile versus ViewOtherProfile. I can think of pros and cons to each approach...</t>
   </si>
   <si>
     <t>Week 8 Activities (last things)
@@ -249,9 +219,6 @@
   </si>
   <si>
     <t>Week 9: Remaining videos + a couple readings, professional dev feedback</t>
-  </si>
-  <si>
-    <t>^^^ Doesn't that servlet mapping still allow JSP's to accessed directly? Do I need to do the mapping?</t>
   </si>
   <si>
     <t>Week 9: Activities - finished activities (with question) but not exercise.  See PW answer re: JSON, probably apply in Exercise rather than in activity.</t>
@@ -273,10 +240,6 @@
   </si>
   <si>
     <t>Indie Project: got ApplicationStartup servlet working.  As far as I can tell it is making the lucen indexes as it should, and it is loading the properties file for the application.  Commented out the lucene index work from individual searches.  Got the method to get income by career working!  (Needs testing, but initial output looks reasonable)</t>
-  </si>
-  <si>
-    <t>Deal with this? -- 13-Apr-2019 06:24:39.625 WARNING [localhost-startStop-2] org.apache.catalina.loader.WebappClassLoaderBase.clearReferencesThreads The web application [incomeexperiences] appears to have started a thread named [C3P0PooledConnectionPoolManager[identityToken-&gt;1hgfbpda2682w263f1q0z|7e4e66]-AdminTaskTimer] but has failed to stop it. This is very likely to create a memory leak. Stack trace of thread:
- java.lang.Object.wait(Native Method)</t>
   </si>
   <si>
     <r>
@@ -323,12 +286,6 @@
     <t>Update project plan. Stats search now displays all charts and associated stories.  Signup functionality and welcome page are drafted but need to add user role and need to refactor/test.</t>
   </si>
   <si>
-    <t>2019-04-26 15:06:52,445 Log4j2-TF-1-RollingFileManager-1 ERROR Error in post-rollover Delete when visiting C:\logs\income_experiences.log java.nio.file.FileSystemException: C:\logs\income_experiences.log: The process cannot access the file because it is being used by another process.</t>
-  </si>
-  <si>
-    <t>^^^ oh hey I just recreated it almost 2 months later!  Maybe it's just occasional</t>
-  </si>
-  <si>
     <t>adding role entity, adding foreign key to db role, debugging breakage (User now needs to be serializable), starting to test, and adding a role upon signup</t>
   </si>
   <si>
@@ -368,34 +325,10 @@
     <t>Added data to database, found software for screencast, fixed a search validation problem.</t>
   </si>
   <si>
-    <t>Weekend</t>
-  </si>
-  <si>
-    <t>Code: focus on testing api and ExperiencesSearch - be smart about priorities</t>
-  </si>
-  <si>
-    <t>Do screencast</t>
-  </si>
-  <si>
-    <t>Do ppt</t>
-  </si>
-  <si>
-    <t>Do rubric/wk 15 - link ppt, video, javadocs… any links needed</t>
-  </si>
-  <si>
-    <t>Close Kelly's comment w/more updates</t>
-  </si>
-  <si>
-    <t>Make javadocs - need to be on GitHub, maybe add link to ReadMe</t>
-  </si>
-  <si>
     <t>worked on presentation (getting to know obs software, making powerpoint, planning flow)</t>
   </si>
   <si>
-    <t>Adding data to deployed application, troubleshooting a crash, and another one. Making the video demo.</t>
-  </si>
-  <si>
-    <t>8:10 - x</t>
+    <t>Adding data to deployed application, troubleshooting a crash, and another one. Making the videos (walk through and some code), updating the readme, project plan, and user stories.  Finishing the PowerPoint (possibly the last unless code improvement is possible tomorrow).</t>
   </si>
 </sst>
 </file>
@@ -805,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C6BDA-F116-40B6-837F-B46593DB9E40}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1029,7 @@
         <v>3.5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1107,7 +1040,7 @@
         <v>3.5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1129,7 +1062,7 @@
         <v>2.5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1140,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1151,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1184,7 +1117,7 @@
         <v>4.5</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1195,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1206,7 +1139,7 @@
         <v>4.5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1217,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1228,7 +1161,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1239,7 +1172,7 @@
         <v>1.5</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1250,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1261,7 +1194,7 @@
         <v>6.5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1283,7 +1216,7 @@
         <v>5.5</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1294,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1305,7 +1238,7 @@
         <v>5.5</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1316,7 +1249,7 @@
         <v>7.5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1327,7 +1260,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1338,7 +1271,7 @@
         <v>1.5</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,7 +1282,7 @@
         <v>5.5</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1360,7 +1293,7 @@
         <v>6.5</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,7 +1304,7 @@
         <v>3.5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1382,7 +1315,7 @@
         <v>6.5</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1393,7 +1326,7 @@
         <v>2.5</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1404,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1415,7 +1348,7 @@
         <v>5</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1426,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1448,7 +1381,7 @@
         <v>4.5</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1459,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1470,7 +1403,7 @@
         <v>3.5</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1481,7 +1414,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1492,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1503,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1514,7 +1447,7 @@
         <v>9</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1536,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,7 +1480,7 @@
         <v>2.5</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1558,7 +1491,7 @@
         <v>3.5</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1569,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1580,7 +1513,7 @@
         <v>9</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1591,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,7 +1535,7 @@
         <v>1.5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1613,7 +1546,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1624,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1635,7 +1568,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1646,7 +1579,7 @@
         <v>5.5</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1657,7 +1590,7 @@
         <v>6.5</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1668,7 +1601,7 @@
         <v>7.5</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1679,7 +1612,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1701,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1712,7 +1645,7 @@
         <v>7</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,18 +1667,18 @@
         <v>5</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43597</v>
       </c>
       <c r="B86">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1756,18 +1689,13 @@
     </row>
     <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="D89" s="2" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
     <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="D91" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="D91" s="9"/>
     </row>
     <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
@@ -1777,132 +1705,54 @@
     </row>
     <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="D94" s="2" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="D95" s="2" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="D96" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="D97" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
-      <c r="D98" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-      <c r="D99" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="D101" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="D105" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="D107" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
-      <c r="D108" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="D110" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="D112" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D114" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="117" spans="4:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="D117" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="120" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    </row>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>